<commit_message>
Udating records 13-01-2025 08:49
</commit_message>
<xml_diff>
--- a/Records.xlsx
+++ b/Records.xlsx
@@ -1,42 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zicooo82/Desktop/معهد الوادي/MyWeRepo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moh_zakria\Desktop\Students URLs\MyWeRepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C1CBC9-02EC-DD4B-8C2D-ED286E84E3F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2527EAC-A115-4F61-AD83-C6CBBA2D0E22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="24240" windowHeight="13140" xr2:uid="{AE619845-176D-4C93-91F5-F1442B84480E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{AE619845-176D-4C93-91F5-F1442B84480E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="179">
   <si>
     <t>Timestamp</t>
   </si>
@@ -558,6 +548,24 @@
   </si>
   <si>
     <t>https://mariamyousef-boop.github.io/this-is-my-page/</t>
+  </si>
+  <si>
+    <t>as20232248@sva.edu.eg</t>
+  </si>
+  <si>
+    <t>https://hoda3225.github.io/my-first-webpage/</t>
+  </si>
+  <si>
+    <t>ys20231357@sva.edu.eg</t>
+  </si>
+  <si>
+    <t>https://goo782.github.io/My-page/</t>
+  </si>
+  <si>
+    <t>ns20232229@sav.edu.eg</t>
+  </si>
+  <si>
+    <t>https://nesmasayed2004.github.io/mypage/</t>
   </si>
 </sst>
 </file>
@@ -623,7 +631,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -871,12 +879,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -954,6 +973,33 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -973,9 +1019,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1013,7 +1059,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1119,7 +1165,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1261,7 +1307,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1269,22 +1315,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97601210-06D1-436F-9FFC-E5C230996E4C}">
-  <dimension ref="A1:E130"/>
+  <dimension ref="A1:E263"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="C130" sqref="C130"/>
+    <sheetView tabSelected="1" topLeftCell="A246" workbookViewId="0">
+      <selection activeCell="C264" sqref="C264"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="119.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="119.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1301,7 +1347,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>45724.771736111114</v>
       </c>
@@ -1314,7 +1360,7 @@
       <c r="D2" s="5"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>45724.772939814815</v>
       </c>
@@ -1327,7 +1373,7 @@
       <c r="D3" s="8"/>
       <c r="E3" s="9"/>
     </row>
-    <row r="4" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>45724.777685185189</v>
       </c>
@@ -1340,7 +1386,7 @@
       <c r="D4" s="5"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>45724.783252314817</v>
       </c>
@@ -1353,7 +1399,7 @@
       <c r="D5" s="8"/>
       <c r="E5" s="9"/>
     </row>
-    <row r="6" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>45724.800636574073</v>
       </c>
@@ -1366,7 +1412,7 @@
       <c r="D6" s="5"/>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>45724.803206018521</v>
       </c>
@@ -1379,7 +1425,7 @@
       <c r="D7" s="8"/>
       <c r="E7" s="9"/>
     </row>
-    <row r="8" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>45724.805752314816</v>
       </c>
@@ -1392,7 +1438,7 @@
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>45724.812673611108</v>
       </c>
@@ -1405,7 +1451,7 @@
       <c r="D9" s="8"/>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>45725.53019675926</v>
       </c>
@@ -1418,7 +1464,7 @@
       <c r="D10" s="5"/>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>45726.039942129632</v>
       </c>
@@ -1431,7 +1477,7 @@
       <c r="D11" s="8"/>
       <c r="E11" s="9"/>
     </row>
-    <row r="12" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>45726.04005787037</v>
       </c>
@@ -1444,7 +1490,7 @@
       <c r="D12" s="5"/>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>45726.356793981482</v>
       </c>
@@ -1457,7 +1503,7 @@
       <c r="D13" s="8"/>
       <c r="E13" s="9"/>
     </row>
-    <row r="14" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>45726.357164351852</v>
       </c>
@@ -1470,7 +1516,7 @@
       <c r="D14" s="5"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>45726.466319444444</v>
       </c>
@@ -1483,7 +1529,7 @@
       <c r="D15" s="8"/>
       <c r="E15" s="9"/>
     </row>
-    <row r="16" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>45726.506782407407</v>
       </c>
@@ -1496,7 +1542,7 @@
       <c r="D16" s="5"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>45726.507210648146</v>
       </c>
@@ -1509,7 +1555,7 @@
       <c r="D17" s="8"/>
       <c r="E17" s="9"/>
     </row>
-    <row r="18" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>45727.02065972222</v>
       </c>
@@ -1522,7 +1568,7 @@
       <c r="D18" s="5"/>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
         <v>45727.022858796299</v>
       </c>
@@ -1533,7 +1579,7 @@
       <c r="D19" s="8"/>
       <c r="E19" s="9"/>
     </row>
-    <row r="20" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>45727.029664351852</v>
       </c>
@@ -1546,7 +1592,7 @@
       <c r="D20" s="5"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
         <v>45727.032870370371</v>
       </c>
@@ -1559,7 +1605,7 @@
       <c r="D21" s="8"/>
       <c r="E21" s="9"/>
     </row>
-    <row r="22" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>45727.033043981479</v>
       </c>
@@ -1572,7 +1618,7 @@
       <c r="D22" s="5"/>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
         <v>45727.039386574077</v>
       </c>
@@ -1585,7 +1631,7 @@
       <c r="D23" s="8"/>
       <c r="E23" s="9"/>
     </row>
-    <row r="24" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>45727.051342592589</v>
       </c>
@@ -1598,7 +1644,7 @@
       <c r="D24" s="5"/>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
         <v>45727.055520833332</v>
       </c>
@@ -1611,7 +1657,7 @@
       <c r="D25" s="8"/>
       <c r="E25" s="9"/>
     </row>
-    <row r="26" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>45727.348298611112</v>
       </c>
@@ -1624,7 +1670,7 @@
       <c r="D26" s="5"/>
       <c r="E26" s="6"/>
     </row>
-    <row r="27" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <v>45727.348761574074</v>
       </c>
@@ -1637,7 +1683,7 @@
       <c r="D27" s="8"/>
       <c r="E27" s="9"/>
     </row>
-    <row r="28" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>45727.550428240742</v>
       </c>
@@ -1650,7 +1696,7 @@
       <c r="D28" s="5"/>
       <c r="E28" s="6"/>
     </row>
-    <row r="29" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <v>45730.132939814815</v>
       </c>
@@ -1663,7 +1709,7 @@
       <c r="D29" s="8"/>
       <c r="E29" s="9"/>
     </row>
-    <row r="30" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>45730.667627314811</v>
       </c>
@@ -1676,7 +1722,7 @@
       <c r="D30" s="5"/>
       <c r="E30" s="6"/>
     </row>
-    <row r="31" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7">
         <v>45730.668043981481</v>
       </c>
@@ -1689,7 +1735,7 @@
       <c r="D31" s="8"/>
       <c r="E31" s="9"/>
     </row>
-    <row r="32" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>45730.692094907405</v>
       </c>
@@ -1702,7 +1748,7 @@
       <c r="D32" s="5"/>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7">
         <v>45731.041458333333</v>
       </c>
@@ -1715,7 +1761,7 @@
       <c r="D33" s="8"/>
       <c r="E33" s="9"/>
     </row>
-    <row r="34" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>45731.042604166665</v>
       </c>
@@ -1728,7 +1774,7 @@
       <c r="D34" s="5"/>
       <c r="E34" s="6"/>
     </row>
-    <row r="35" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7">
         <v>45731.383217592593</v>
       </c>
@@ -1741,7 +1787,7 @@
       <c r="D35" s="8"/>
       <c r="E35" s="9"/>
     </row>
-    <row r="36" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>45731.89230324074</v>
       </c>
@@ -1754,7 +1800,7 @@
       <c r="D36" s="5"/>
       <c r="E36" s="6"/>
     </row>
-    <row r="37" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="7">
         <v>45731.892442129632</v>
       </c>
@@ -1767,7 +1813,7 @@
       <c r="D37" s="8"/>
       <c r="E37" s="9"/>
     </row>
-    <row r="38" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>45731.893680555557</v>
       </c>
@@ -1780,7 +1826,7 @@
       <c r="D38" s="5"/>
       <c r="E38" s="6"/>
     </row>
-    <row r="39" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="7">
         <v>45731.893842592595</v>
       </c>
@@ -1793,7 +1839,7 @@
       <c r="D39" s="8"/>
       <c r="E39" s="9"/>
     </row>
-    <row r="40" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>45731.895567129628</v>
       </c>
@@ -1806,7 +1852,7 @@
       <c r="D40" s="5"/>
       <c r="E40" s="6"/>
     </row>
-    <row r="41" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="7">
         <v>45733.789525462962</v>
       </c>
@@ -1819,7 +1865,7 @@
       <c r="D41" s="8"/>
       <c r="E41" s="9"/>
     </row>
-    <row r="42" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>45733.795115740744</v>
       </c>
@@ -1832,7 +1878,7 @@
       <c r="D42" s="5"/>
       <c r="E42" s="6"/>
     </row>
-    <row r="43" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7">
         <v>45733.800370370373</v>
       </c>
@@ -1845,7 +1891,7 @@
       <c r="D43" s="8"/>
       <c r="E43" s="9"/>
     </row>
-    <row r="44" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>45733.805578703701</v>
       </c>
@@ -1858,7 +1904,7 @@
       <c r="D44" s="5"/>
       <c r="E44" s="6"/>
     </row>
-    <row r="45" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7">
         <v>45733.80641203704</v>
       </c>
@@ -1871,7 +1917,7 @@
       <c r="D45" s="8"/>
       <c r="E45" s="9"/>
     </row>
-    <row r="46" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>45733.816261574073</v>
       </c>
@@ -1884,7 +1930,7 @@
       <c r="D46" s="5"/>
       <c r="E46" s="6"/>
     </row>
-    <row r="47" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="7">
         <v>45735.574652777781</v>
       </c>
@@ -1897,7 +1943,7 @@
       <c r="D47" s="8"/>
       <c r="E47" s="9"/>
     </row>
-    <row r="48" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>45733.827337962961</v>
       </c>
@@ -1910,7 +1956,7 @@
       <c r="D48" s="5"/>
       <c r="E48" s="6"/>
     </row>
-    <row r="49" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="7">
         <v>45733.838587962964</v>
       </c>
@@ -1923,7 +1969,7 @@
       <c r="D49" s="8"/>
       <c r="E49" s="9"/>
     </row>
-    <row r="50" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>45733.851712962962</v>
       </c>
@@ -1936,7 +1982,7 @@
       <c r="D50" s="5"/>
       <c r="E50" s="6"/>
     </row>
-    <row r="51" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="7">
         <v>45733.881053240744</v>
       </c>
@@ -1949,7 +1995,7 @@
       <c r="D51" s="8"/>
       <c r="E51" s="9"/>
     </row>
-    <row r="52" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>45735.546041666668</v>
       </c>
@@ -1962,7 +2008,7 @@
       <c r="D52" s="5"/>
       <c r="E52" s="6"/>
     </row>
-    <row r="53" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="7">
         <v>45733.974374999998</v>
       </c>
@@ -1975,7 +2021,7 @@
       <c r="D53" s="8"/>
       <c r="E53" s="9"/>
     </row>
-    <row r="54" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
         <v>45733.987372685187</v>
       </c>
@@ -1988,7 +2034,7 @@
       <c r="D54" s="5"/>
       <c r="E54" s="6"/>
     </row>
-    <row r="55" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="7">
         <v>45733.991678240738</v>
       </c>
@@ -2001,7 +2047,7 @@
       <c r="D55" s="8"/>
       <c r="E55" s="9"/>
     </row>
-    <row r="56" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4">
         <v>45734.08734953704</v>
       </c>
@@ -2014,7 +2060,7 @@
       <c r="D56" s="5"/>
       <c r="E56" s="6"/>
     </row>
-    <row r="57" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="7">
         <v>45734.128171296295</v>
       </c>
@@ -2027,7 +2073,7 @@
       <c r="D57" s="8"/>
       <c r="E57" s="9"/>
     </row>
-    <row r="58" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
         <v>45734.495439814818</v>
       </c>
@@ -2040,7 +2086,7 @@
       <c r="D58" s="5"/>
       <c r="E58" s="6"/>
     </row>
-    <row r="59" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="7">
         <v>45734.552002314813</v>
       </c>
@@ -2053,7 +2099,7 @@
       <c r="D59" s="8"/>
       <c r="E59" s="9"/>
     </row>
-    <row r="60" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
         <v>45734.606840277775</v>
       </c>
@@ -2066,7 +2112,7 @@
       <c r="D60" s="5"/>
       <c r="E60" s="6"/>
     </row>
-    <row r="61" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="7">
         <v>45734.612662037034</v>
       </c>
@@ -2079,7 +2125,7 @@
       <c r="D61" s="8"/>
       <c r="E61" s="9"/>
     </row>
-    <row r="62" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4">
         <v>45734.63653935185</v>
       </c>
@@ -2092,7 +2138,7 @@
       <c r="D62" s="5"/>
       <c r="E62" s="6"/>
     </row>
-    <row r="63" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="7">
         <v>45734.719652777778</v>
       </c>
@@ -2105,7 +2151,7 @@
       <c r="D63" s="8"/>
       <c r="E63" s="9"/>
     </row>
-    <row r="64" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4">
         <v>45734.721446759257</v>
       </c>
@@ -2118,7 +2164,7 @@
       <c r="D64" s="5"/>
       <c r="E64" s="6"/>
     </row>
-    <row r="65" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="7">
         <v>45734.725555555553</v>
       </c>
@@ -2131,7 +2177,7 @@
       <c r="D65" s="8"/>
       <c r="E65" s="9"/>
     </row>
-    <row r="66" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="4">
         <v>45734.728935185187</v>
       </c>
@@ -2144,7 +2190,7 @@
       <c r="D66" s="5"/>
       <c r="E66" s="6"/>
     </row>
-    <row r="67" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="7">
         <v>45734.863935185182</v>
       </c>
@@ -2157,7 +2203,7 @@
       <c r="D67" s="8"/>
       <c r="E67" s="9"/>
     </row>
-    <row r="68" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="4">
         <v>45735.164502314816</v>
       </c>
@@ -2170,7 +2216,7 @@
       <c r="D68" s="5"/>
       <c r="E68" s="6"/>
     </row>
-    <row r="69" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="7">
         <v>45735.229097222225</v>
       </c>
@@ -2183,7 +2229,7 @@
       <c r="D69" s="8"/>
       <c r="E69" s="9"/>
     </row>
-    <row r="70" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="4">
         <v>45735.262106481481</v>
       </c>
@@ -2196,7 +2242,7 @@
       <c r="D70" s="5"/>
       <c r="E70" s="6"/>
     </row>
-    <row r="71" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="7">
         <v>45735.341168981482</v>
       </c>
@@ -2209,7 +2255,7 @@
       <c r="D71" s="8"/>
       <c r="E71" s="9"/>
     </row>
-    <row r="72" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="4">
         <v>45735.395312499997</v>
       </c>
@@ -2222,7 +2268,7 @@
       <c r="D72" s="5"/>
       <c r="E72" s="6"/>
     </row>
-    <row r="73" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="7">
         <v>45735.414930555555</v>
       </c>
@@ -2235,7 +2281,7 @@
       <c r="D73" s="8"/>
       <c r="E73" s="9"/>
     </row>
-    <row r="74" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="4">
         <v>45735.517326388886</v>
       </c>
@@ -2248,7 +2294,7 @@
       <c r="D74" s="5"/>
       <c r="E74" s="6"/>
     </row>
-    <row r="75" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="7">
         <v>45735.634039351855</v>
       </c>
@@ -2261,7 +2307,7 @@
       <c r="D75" s="8"/>
       <c r="E75" s="9"/>
     </row>
-    <row r="76" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="4">
         <v>45735.653171296297</v>
       </c>
@@ -2274,7 +2320,7 @@
       <c r="D76" s="5"/>
       <c r="E76" s="6"/>
     </row>
-    <row r="77" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="7">
         <v>45735.656875000001</v>
       </c>
@@ -2287,7 +2333,7 @@
       <c r="D77" s="8"/>
       <c r="E77" s="9"/>
     </row>
-    <row r="78" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="4">
         <v>45735.669131944444</v>
       </c>
@@ -2300,7 +2346,7 @@
       <c r="D78" s="5"/>
       <c r="E78" s="6"/>
     </row>
-    <row r="79" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="7">
         <v>45735.683749999997</v>
       </c>
@@ -2313,7 +2359,7 @@
       <c r="D79" s="8"/>
       <c r="E79" s="9"/>
     </row>
-    <row r="80" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="4">
         <v>45735.722696759258</v>
       </c>
@@ -2326,7 +2372,7 @@
       <c r="D80" s="5"/>
       <c r="E80" s="6"/>
     </row>
-    <row r="81" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="7">
         <v>45735.73709490741</v>
       </c>
@@ -2339,7 +2385,7 @@
       <c r="D81" s="8"/>
       <c r="E81" s="9"/>
     </row>
-    <row r="82" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="4">
         <v>45735.791226851848</v>
       </c>
@@ -2352,7 +2398,7 @@
       <c r="D82" s="5"/>
       <c r="E82" s="6"/>
     </row>
-    <row r="83" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="7">
         <v>45735.815532407411</v>
       </c>
@@ -2365,7 +2411,7 @@
       <c r="D83" s="8"/>
       <c r="E83" s="9"/>
     </row>
-    <row r="84" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="4">
         <v>45735.83017361111</v>
       </c>
@@ -2378,7 +2424,7 @@
       <c r="D84" s="5"/>
       <c r="E84" s="6"/>
     </row>
-    <row r="85" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="7">
         <v>45735.904293981483</v>
       </c>
@@ -2391,7 +2437,7 @@
       <c r="D85" s="8"/>
       <c r="E85" s="9"/>
     </row>
-    <row r="86" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="4">
         <v>45735.916076388887</v>
       </c>
@@ -2404,7 +2450,7 @@
       <c r="D86" s="5"/>
       <c r="E86" s="6"/>
     </row>
-    <row r="87" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="7">
         <v>45735.931064814817</v>
       </c>
@@ -2417,7 +2463,7 @@
       <c r="D87" s="8"/>
       <c r="E87" s="9"/>
     </row>
-    <row r="88" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="4">
         <v>45735.954722222225</v>
       </c>
@@ -2430,7 +2476,7 @@
       <c r="D88" s="5"/>
       <c r="E88" s="6"/>
     </row>
-    <row r="89" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="7">
         <v>45736.216805555552</v>
       </c>
@@ -2443,7 +2489,7 @@
       <c r="D89" s="8"/>
       <c r="E89" s="9"/>
     </row>
-    <row r="90" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="4">
         <v>45736.221365740741</v>
       </c>
@@ -2456,7 +2502,7 @@
       <c r="D90" s="5"/>
       <c r="E90" s="6"/>
     </row>
-    <row r="91" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="7">
         <v>45736.383368055554</v>
       </c>
@@ -2469,7 +2515,7 @@
       <c r="D91" s="8"/>
       <c r="E91" s="9"/>
     </row>
-    <row r="92" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="4">
         <v>45736.435949074075</v>
       </c>
@@ -2482,7 +2528,7 @@
       <c r="D92" s="5"/>
       <c r="E92" s="6"/>
     </row>
-    <row r="93" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="7">
         <v>45736.531006944446</v>
       </c>
@@ -2495,7 +2541,7 @@
       <c r="D93" s="8"/>
       <c r="E93" s="9"/>
     </row>
-    <row r="94" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="4">
         <v>45736.532453703701</v>
       </c>
@@ -2508,7 +2554,7 @@
       <c r="D94" s="5"/>
       <c r="E94" s="6"/>
     </row>
-    <row r="95" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="7">
         <v>45736.622372685182</v>
       </c>
@@ -2521,7 +2567,7 @@
       <c r="D95" s="8"/>
       <c r="E95" s="9"/>
     </row>
-    <row r="96" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="4">
         <v>45736.630844907406</v>
       </c>
@@ -2534,7 +2580,7 @@
       <c r="D96" s="5"/>
       <c r="E96" s="6"/>
     </row>
-    <row r="97" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="7">
         <v>45736.789652777778</v>
       </c>
@@ -2547,7 +2593,7 @@
       <c r="D97" s="8"/>
       <c r="E97" s="9"/>
     </row>
-    <row r="98" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="4">
         <v>45736.954583333332</v>
       </c>
@@ -2560,7 +2606,7 @@
       <c r="D98" s="5"/>
       <c r="E98" s="6"/>
     </row>
-    <row r="99" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="7">
         <v>45736.958553240744</v>
       </c>
@@ -2573,7 +2619,7 @@
       <c r="D99" s="8"/>
       <c r="E99" s="9"/>
     </row>
-    <row r="100" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="4">
         <v>45736.958796296298</v>
       </c>
@@ -2586,7 +2632,7 @@
       <c r="D100" s="5"/>
       <c r="E100" s="6"/>
     </row>
-    <row r="101" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="7">
         <v>45737.594444444447</v>
       </c>
@@ -2599,7 +2645,7 @@
       <c r="D101" s="8"/>
       <c r="E101" s="9"/>
     </row>
-    <row r="102" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="4">
         <v>45737.594560185185</v>
       </c>
@@ -2612,7 +2658,7 @@
       <c r="D102" s="5"/>
       <c r="E102" s="6"/>
     </row>
-    <row r="103" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="7">
         <v>45737.594675925924</v>
       </c>
@@ -2625,7 +2671,7 @@
       <c r="D103" s="8"/>
       <c r="E103" s="9"/>
     </row>
-    <row r="104" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="4">
         <v>45737.625115740739</v>
       </c>
@@ -2638,7 +2684,7 @@
       <c r="D104" s="5"/>
       <c r="E104" s="6"/>
     </row>
-    <row r="105" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="7">
         <v>45737.638344907406</v>
       </c>
@@ -2651,7 +2697,7 @@
       <c r="D105" s="8"/>
       <c r="E105" s="9"/>
     </row>
-    <row r="106" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="4">
         <v>45737.638645833336</v>
       </c>
@@ -2664,7 +2710,7 @@
       <c r="D106" s="5"/>
       <c r="E106" s="6"/>
     </row>
-    <row r="107" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="7">
         <v>45737.662002314813</v>
       </c>
@@ -2677,7 +2723,7 @@
       <c r="D107" s="8"/>
       <c r="E107" s="9"/>
     </row>
-    <row r="108" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="4">
         <v>45737.693680555552</v>
       </c>
@@ -2690,7 +2736,7 @@
       <c r="D108" s="5"/>
       <c r="E108" s="6"/>
     </row>
-    <row r="109" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="7">
         <v>45737.693831018521</v>
       </c>
@@ -2703,7 +2749,7 @@
       <c r="D109" s="8"/>
       <c r="E109" s="9"/>
     </row>
-    <row r="110" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="4">
         <v>45737.7031712963</v>
       </c>
@@ -2716,7 +2762,7 @@
       <c r="D110" s="5"/>
       <c r="E110" s="6"/>
     </row>
-    <row r="111" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="7">
         <v>45737.703530092593</v>
       </c>
@@ -2729,7 +2775,7 @@
       <c r="D111" s="8"/>
       <c r="E111" s="9"/>
     </row>
-    <row r="112" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="4">
         <v>45737.87636574074</v>
       </c>
@@ -2742,7 +2788,7 @@
       <c r="D112" s="5"/>
       <c r="E112" s="6"/>
     </row>
-    <row r="113" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="7">
         <v>45737.876574074071</v>
       </c>
@@ -2755,7 +2801,7 @@
       <c r="D113" s="8"/>
       <c r="E113" s="9"/>
     </row>
-    <row r="114" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="4">
         <v>45737.987118055556</v>
       </c>
@@ -2768,7 +2814,7 @@
       <c r="D114" s="5"/>
       <c r="E114" s="6"/>
     </row>
-    <row r="115" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="7">
         <v>45738.049212962964</v>
       </c>
@@ -2781,7 +2827,7 @@
       <c r="D115" s="8"/>
       <c r="E115" s="9"/>
     </row>
-    <row r="116" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="4">
         <v>45738.637048611112</v>
       </c>
@@ -2794,7 +2840,7 @@
       <c r="D116" s="5"/>
       <c r="E116" s="6"/>
     </row>
-    <row r="117" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="7">
         <v>45738.637326388889</v>
       </c>
@@ -2807,7 +2853,7 @@
       <c r="D117" s="8"/>
       <c r="E117" s="9"/>
     </row>
-    <row r="118" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="4">
         <v>45738.740254629629</v>
       </c>
@@ -2820,7 +2866,7 @@
       <c r="D118" s="5"/>
       <c r="E118" s="6"/>
     </row>
-    <row r="119" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="7">
         <v>45738.740439814814</v>
       </c>
@@ -2833,7 +2879,7 @@
       <c r="D119" s="8"/>
       <c r="E119" s="9"/>
     </row>
-    <row r="120" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="4">
         <v>45738.741099537037</v>
       </c>
@@ -2846,7 +2892,7 @@
       <c r="D120" s="5"/>
       <c r="E120" s="6"/>
     </row>
-    <row r="121" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="7">
         <v>45739.096574074072</v>
       </c>
@@ -2859,7 +2905,7 @@
       <c r="D121" s="8"/>
       <c r="E121" s="9"/>
     </row>
-    <row r="122" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="4">
         <v>45739.616539351853</v>
       </c>
@@ -2872,7 +2918,7 @@
       <c r="D122" s="5"/>
       <c r="E122" s="6"/>
     </row>
-    <row r="123" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="10">
         <v>45740.519872685189</v>
       </c>
@@ -2885,7 +2931,7 @@
       <c r="D123" s="11"/>
       <c r="E123" s="12"/>
     </row>
-    <row r="124" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B124" s="17" t="s">
         <v>161</v>
       </c>
@@ -2893,7 +2939,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B125" s="15" t="s">
         <v>163</v>
       </c>
@@ -2901,7 +2947,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="126" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B126" s="17" t="s">
         <v>165</v>
       </c>
@@ -2909,7 +2955,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="127" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B127" s="24" t="s">
         <v>77</v>
       </c>
@@ -2917,7 +2963,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B128" s="24" t="s">
         <v>168</v>
       </c>
@@ -2925,7 +2971,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>170</v>
       </c>
@@ -2933,12 +2979,1074 @@
         <v>169</v>
       </c>
     </row>
-    <row r="130" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B130" t="s">
         <v>171</v>
       </c>
       <c r="C130" t="s">
         <v>172</v>
+      </c>
+    </row>
+    <row r="131" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B131" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C131" s="28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B132" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C132" s="30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="133" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B133" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C133" s="31">
+        <v>30509051400865</v>
+      </c>
+    </row>
+    <row r="134" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B134" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C134" s="32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="135" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B135" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C135" s="27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="136" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B136" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C136" s="30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="137" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B137" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C137" s="31">
+        <v>20233360</v>
+      </c>
+    </row>
+    <row r="138" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B138" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C138" s="32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="139" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B139" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C139" s="31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="140" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B140" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C140" s="32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="141" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B141" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C141" s="28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="142" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B142" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C142" s="30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="143" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B143" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C143" s="31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="144" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B144" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C144" s="30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="145" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B145" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C145" s="31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="146" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B146" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C146" s="30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="147" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B147" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C147" s="28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="148" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B148" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C148" s="8"/>
+    </row>
+    <row r="149" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B149" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C149" s="28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="150" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B150" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C150" s="30">
+        <v>20233360</v>
+      </c>
+    </row>
+    <row r="151" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B151" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C151" s="31">
+        <v>20233360</v>
+      </c>
+    </row>
+    <row r="152" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B152" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C152" s="29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="153" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B153" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C153" s="28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="154" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B154" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C154" s="32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="155" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B155" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C155" s="28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="156" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B156" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C156" s="32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="157" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B157" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C157" s="28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="158" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B158" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C158" s="32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="159" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B159" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C159" s="28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="160" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B160" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C160" s="32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="161" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B161" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C161" s="28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="162" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B162" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C162" s="29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="163" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B163" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C163" s="27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="164" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B164" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C164" s="32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="165" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B165" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C165" s="28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="166" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B166" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C166" s="32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="167" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B167" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C167" s="28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="168" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B168" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C168" s="32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="169" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B169" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C169" s="27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="170" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B170" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C170" s="29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="171" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B171" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C171" s="28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="172" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B172" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C172" s="29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="173" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B173" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C173" s="28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="174" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B174" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C174" s="29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="175" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B175" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C175" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="176" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B176" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C176" s="32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="177" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B177" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C177" s="27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="178" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B178" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C178" s="32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="179" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B179" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C179" s="28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="180" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B180" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C180" s="29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="181" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B181" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C181" s="28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="182" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B182" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C182" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="183" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B183" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C183" s="28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="184" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B184" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C184" s="32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="185" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B185" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C185" s="27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="186" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B186" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C186" s="32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="187" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B187" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C187" s="31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="188" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B188" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C188" s="32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="189" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B189" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="C189" s="28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="190" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B190" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="C190" s="30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="191" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B191" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C191" s="28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="192" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B192" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C192" s="32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="193" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B193" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C193" s="28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="194" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B194" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C194" s="32" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="195" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B195" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C195" s="28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="196" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B196" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C196" s="32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="197" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B197" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="C197" s="27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="198" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B198" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C198" s="29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="199" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B199" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C199" s="28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="200" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B200" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C200" s="32" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="201" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B201" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="C201" s="28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="202" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B202" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="C202" s="32" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="203" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B203" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C203" s="28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="204" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B204" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="C204" s="30" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="205" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B205" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="C205" s="28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="206" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B206" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="C206" s="32" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="207" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B207" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="C207" s="28" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="208" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B208" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="C208" s="32" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="209" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B209" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="C209" s="28" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="210" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B210" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="C210" s="32" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="211" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B211" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="C211" s="28" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="212" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B212" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="C212" s="30" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="213" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B213" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="C213" s="27" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="214" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B214" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="C214" s="29" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="215" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B215" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="C215" s="28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="216" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B216" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="C216" s="32" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="217" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B217" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="C217" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="218" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B218" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C218" s="32" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="219" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B219" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="C219" s="28" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="220" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B220" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="C220" s="30" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="221" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B221" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="C221" s="28" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="222" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B222" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="C222" s="32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="223" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B223" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="C223" s="28" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="224" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B224" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="C224" s="29" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="225" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B225" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="C225" s="28" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="226" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B226" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="C226" s="32" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="227" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B227" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="C227" s="28" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="228" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B228" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="C228" s="32" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="229" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B229" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="C229" s="28" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="230" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B230" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="C230" s="32" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="231" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B231" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="C231" s="28" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="232" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B232" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="C232" s="32" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="233" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B233" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="C233" s="28" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="234" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B234" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="C234" s="32" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="235" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B235" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="C235" s="28" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="236" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B236" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C236" s="32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="237" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B237" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="C237" s="27" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="238" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B238" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="C238" s="32" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="239" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B239" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="C239" s="28" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="240" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B240" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="C240" s="32" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="241" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B241" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="C241" s="28" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="242" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B242" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="C242" s="32" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="243" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B243" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="C243" s="28" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="244" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B244" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="C244" s="32" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="245" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B245" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="C245" s="28" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="246" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B246" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="C246" s="32" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="247" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B247" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="C247" s="28" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="248" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B248" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="C248" s="32" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="249" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B249" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="C249" s="28" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="250" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B250" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="C250" s="32" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="251" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B251" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="C251" s="27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="252" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B252" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="C252" s="32" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="253" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B253" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="C253" s="28" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="254" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B254" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="C254" s="32" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="255" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B255" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="C255" s="28" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="256" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B256" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C256" s="32" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="257" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B257" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="C257" s="28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="258" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B258" s="29" t="s">
+        <v>170</v>
+      </c>
+      <c r="C258" s="32" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="259" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B259" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C259" s="28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="260" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B260" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C260" s="32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="261" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B261" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="C261" s="28" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="262" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B262" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="C262" s="34" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="263" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B263" s="35" t="s">
+        <v>177</v>
+      </c>
+      <c r="C263" s="26" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -3034,6 +4142,1956 @@
     <hyperlink ref="C126" r:id="rId89" xr:uid="{E3F3C8CD-7664-4ADE-98D7-154B4479A917}"/>
     <hyperlink ref="C127" r:id="rId90" xr:uid="{BA0D527C-0E33-45F6-8CD2-EC9AE331D884}"/>
     <hyperlink ref="C128" r:id="rId91" xr:uid="{27326168-368F-455C-B8CA-852A1348805F}"/>
+    <hyperlink ref="C131" r:id="rId92" xr:uid="{14225C5E-B7BD-49C6-86AA-AFB391EB8E37}"/>
+    <hyperlink ref="C134" r:id="rId93" xr:uid="{32957B8F-DB3C-4F52-8B42-D4BBEB87DBE9}"/>
+    <hyperlink ref="C138" r:id="rId94" xr:uid="{04618E1E-8396-41A2-BBCD-D991F77023F9}"/>
+    <hyperlink ref="C140" r:id="rId95" xr:uid="{96987C03-6C37-414C-9120-2A9714D06B1C}"/>
+    <hyperlink ref="C141" r:id="rId96" xr:uid="{6332ABA4-BB09-4A1E-A912-45ECFA97D184}"/>
+    <hyperlink ref="C147" r:id="rId97" xr:uid="{A634D200-5823-48B0-BC32-A4BED6E2E506}"/>
+    <hyperlink ref="C149" r:id="rId98" xr:uid="{2407C056-4360-409E-B4BA-6AB5B8595856}"/>
+    <hyperlink ref="C153" r:id="rId99" xr:uid="{8AB0AA49-4B2D-4D37-88C0-818EE05708DF}"/>
+    <hyperlink ref="C154" r:id="rId100" xr:uid="{250D35DE-8E69-4833-8FC2-1B455E8436F5}"/>
+    <hyperlink ref="C155" r:id="rId101" xr:uid="{C9598387-4A22-4D28-A4E3-F065D0F94BEE}"/>
+    <hyperlink ref="C156" r:id="rId102" xr:uid="{BEB7ADC7-0023-4A40-AA34-BC120E04B9AA}"/>
+    <hyperlink ref="C157" r:id="rId103" xr:uid="{ED919C9F-AED8-49C0-A099-3CB8973442DA}"/>
+    <hyperlink ref="C158" r:id="rId104" xr:uid="{423FCCA3-0875-4113-BEA8-52DE51F80E57}"/>
+    <hyperlink ref="C159" r:id="rId105" xr:uid="{5E8F0970-81DB-400E-8287-65F12AE3A2DE}"/>
+    <hyperlink ref="C160" r:id="rId106" xr:uid="{25A77503-A007-47C4-8016-3524337ABE29}"/>
+    <hyperlink ref="C161" r:id="rId107" xr:uid="{FCB1BB1F-588E-4D67-97E2-90021FBAB9E7}"/>
+    <hyperlink ref="C164" r:id="rId108" xr:uid="{A53E6AB1-B6D7-4E89-9057-228FC67F2874}"/>
+    <hyperlink ref="C165" r:id="rId109" xr:uid="{F13B9639-BA14-434A-8117-7D41E9772A6D}"/>
+    <hyperlink ref="C166" r:id="rId110" xr:uid="{26944A19-2D7D-4CF9-877A-82A6AF3BB535}"/>
+    <hyperlink ref="C167" r:id="rId111" xr:uid="{8F8E2E15-9666-4D6C-8664-732778A22B2F}"/>
+    <hyperlink ref="C168" r:id="rId112" xr:uid="{D993C5A1-72D3-4978-AE37-4ACB911DF3DB}"/>
+    <hyperlink ref="C171" r:id="rId113" xr:uid="{2784E194-CBB6-45F7-B1C1-6C038F235E85}"/>
+    <hyperlink ref="C173" r:id="rId114" xr:uid="{DA7B7ED9-23B3-4857-8AC1-D17DD7636BF1}"/>
+    <hyperlink ref="C175" r:id="rId115" xr:uid="{FB699941-5324-46F4-B7F6-EC1AAB02D83D}"/>
+    <hyperlink ref="C176" r:id="rId116" xr:uid="{03D2BC55-4C3C-426E-A9F2-D3D9E0F44B8A}"/>
+    <hyperlink ref="C178" r:id="rId117" xr:uid="{C7BAA3EE-45BE-4F71-8E10-0D41D75C7D03}"/>
+    <hyperlink ref="C179" r:id="rId118" xr:uid="{13861B14-C0CE-4426-AC3E-21DF973CE63D}"/>
+    <hyperlink ref="C181" r:id="rId119" xr:uid="{7B7D1175-DC1B-4493-9041-2B37EB4D19AA}"/>
+    <hyperlink ref="C182" r:id="rId120" xr:uid="{BA6E4306-90D7-47A5-A7D8-8792C7984186}"/>
+    <hyperlink ref="C183" r:id="rId121" xr:uid="{D930B4B3-2AA6-4855-A7E1-B27723648EB4}"/>
+    <hyperlink ref="C184" r:id="rId122" xr:uid="{B3558EE9-D82A-473A-91C7-8EC21EBB0587}"/>
+    <hyperlink ref="C186" r:id="rId123" xr:uid="{BC198CA1-EDAB-482F-8D2E-FD8A1FA2BE3B}"/>
+    <hyperlink ref="C188" r:id="rId124" xr:uid="{0A7786C8-C00E-4C0A-BE42-6940F41702F9}"/>
+    <hyperlink ref="C189" r:id="rId125" xr:uid="{1F8488F3-5AB4-4292-99ED-5B9DEA9339B8}"/>
+    <hyperlink ref="C191" r:id="rId126" xr:uid="{D084E017-9652-4BCC-B807-7FC98E313ADA}"/>
+    <hyperlink ref="C192" r:id="rId127" xr:uid="{3FCF43E2-8A67-475C-A54E-100AA5893C99}"/>
+    <hyperlink ref="C193" r:id="rId128" xr:uid="{B3CF6434-FB7E-478C-AC6A-08D68BE25A97}"/>
+    <hyperlink ref="C194" r:id="rId129" xr:uid="{D8301C01-B6A1-436E-BE87-6D50272D0A2B}"/>
+    <hyperlink ref="C195" r:id="rId130" xr:uid="{13766ED0-555E-440E-A7CF-62FE285EC3C0}"/>
+    <hyperlink ref="C196" r:id="rId131" xr:uid="{5908520D-AE33-43AD-A3A5-86EBBA94D7BA}"/>
+    <hyperlink ref="C199" r:id="rId132" xr:uid="{BD570479-CECC-43A3-80C3-E466905D211B}"/>
+    <hyperlink ref="C200" r:id="rId133" xr:uid="{DC140F46-EAEE-49E8-86DC-DFE09CDBCD5E}"/>
+    <hyperlink ref="C201" r:id="rId134" xr:uid="{5508B6FD-40E8-4638-93B4-43A14BC1E7D5}"/>
+    <hyperlink ref="C202" r:id="rId135" xr:uid="{48CA729B-3886-4857-9683-8A41706D74B0}"/>
+    <hyperlink ref="C203" r:id="rId136" xr:uid="{F7FFD695-3573-43F6-9522-2D9A07BE7F3C}"/>
+    <hyperlink ref="C205" r:id="rId137" display="https://rahma5555.github.io/roro00/" xr:uid="{2EF0D4DE-1427-4630-9CCD-2F1F66305D0A}"/>
+    <hyperlink ref="C206" r:id="rId138" xr:uid="{D2054565-FD4D-4872-937F-A434528B45C8}"/>
+    <hyperlink ref="C207" r:id="rId139" xr:uid="{D1708153-4D09-4BD8-899A-CB9B9FEEE278}"/>
+    <hyperlink ref="C208" r:id="rId140" xr:uid="{AB34F1A6-76B8-4C6B-99F5-665D19ED8892}"/>
+    <hyperlink ref="C209" r:id="rId141" xr:uid="{CE602436-2E0A-40C0-A2A1-6E20C7918D1C}"/>
+    <hyperlink ref="C210" r:id="rId142" xr:uid="{4BF9E4EF-67C4-4DFB-969B-D0440AE03ADB}"/>
+    <hyperlink ref="C211" r:id="rId143" xr:uid="{7082CB31-610E-43EF-8643-D416C81841D3}"/>
+    <hyperlink ref="C215" r:id="rId144" xr:uid="{93AE67AC-8601-4DB6-ADF9-09383D3E5A27}"/>
+    <hyperlink ref="C216" r:id="rId145" xr:uid="{A1701B05-7572-47AE-9E5E-96978D821923}"/>
+    <hyperlink ref="C217" r:id="rId146" xr:uid="{2BA08A41-A9BB-4EBA-9757-1B8262CB1848}"/>
+    <hyperlink ref="C218" r:id="rId147" xr:uid="{58110AEF-7B4E-4C66-8B98-7C4EF8EC0D57}"/>
+    <hyperlink ref="C219" r:id="rId148" display="https://loloah20.githup.io/sva20/" xr:uid="{DAC1F688-ECAD-42C7-943E-63DC70C49950}"/>
+    <hyperlink ref="C221" r:id="rId149" xr:uid="{EA723097-6D62-412F-A756-DD027F91B1A5}"/>
+    <hyperlink ref="C222" r:id="rId150" xr:uid="{BC69EDDB-C9A6-427B-BEE9-FD64E4621C8E}"/>
+    <hyperlink ref="C223" r:id="rId151" xr:uid="{5A81CA0B-DD86-4996-997B-ADB7B883713C}"/>
+    <hyperlink ref="C225" r:id="rId152" xr:uid="{A6C05884-AB6D-46A5-9B45-79195B8D854A}"/>
+    <hyperlink ref="C226" r:id="rId153" display="https://abdullahmahmoud20234326.github.io/myweb/" xr:uid="{E487F24C-31E3-4F40-AC47-62759D5D054B}"/>
+    <hyperlink ref="C227" r:id="rId154" xr:uid="{B6621E51-F004-4E17-8D25-328B946FD3BB}"/>
+    <hyperlink ref="C228" r:id="rId155" xr:uid="{8CAE9522-9864-4A3C-8A9A-B479EECACE63}"/>
+    <hyperlink ref="C229" r:id="rId156" xr:uid="{EE77A9AB-D20A-4AAF-A084-1159351150EB}"/>
+    <hyperlink ref="C230" r:id="rId157" xr:uid="{BE3BF1DB-0DF0-4967-A5D2-F76BA18A6416}"/>
+    <hyperlink ref="C231" r:id="rId158" xr:uid="{2A63E44A-D7AE-4805-A85B-E83457D922D3}"/>
+    <hyperlink ref="C232" r:id="rId159" xr:uid="{C592C7B0-0457-416C-865D-C22B058D5EE0}"/>
+    <hyperlink ref="C233" r:id="rId160" display="https://basant1512006.github.io/basant-walid/" xr:uid="{02947F82-58DE-45A5-B7E6-E6E4BF451D12}"/>
+    <hyperlink ref="C234" r:id="rId161" xr:uid="{9B37BF0E-136A-4B76-B394-4FCBD71CDA18}"/>
+    <hyperlink ref="C235" r:id="rId162" xr:uid="{5906300B-8E57-4281-8263-1712A23FFBA1}"/>
+    <hyperlink ref="C236" r:id="rId163" xr:uid="{358A3FE3-9433-40E6-8410-0E28B3B8DB6D}"/>
+    <hyperlink ref="C238" r:id="rId164" display="https://basant1512006.github.io/Rofida-gehad/" xr:uid="{3B00A136-0367-4FEC-8164-BC159620AE28}"/>
+    <hyperlink ref="C239" r:id="rId165" xr:uid="{6C15C93E-F838-4F23-93C9-927294F21285}"/>
+    <hyperlink ref="C240" r:id="rId166" xr:uid="{CE60375C-D8CA-44DD-9961-83F965CC6791}"/>
+    <hyperlink ref="C241" r:id="rId167" xr:uid="{AEBDE4AB-9C66-48DE-BCD0-FC9639AEC8F3}"/>
+    <hyperlink ref="C242" r:id="rId168" xr:uid="{E44C41FF-4CA1-41D2-8F3E-A0BB7305DBC2}"/>
+    <hyperlink ref="C243" r:id="rId169" xr:uid="{21AF7C4F-149E-42D6-A805-387A559640D2}"/>
+    <hyperlink ref="C244" r:id="rId170" xr:uid="{B9057F45-FF97-4864-B9B2-2D1DF2BA092E}"/>
+    <hyperlink ref="C245" r:id="rId171" xr:uid="{CDF24FCA-1BBD-4D2F-A3E4-3AFCD35FE6DC}"/>
+    <hyperlink ref="C246" r:id="rId172" xr:uid="{189C1E80-CD6A-40B8-B513-F7DB0DDD378B}"/>
+    <hyperlink ref="C247" r:id="rId173" xr:uid="{C1F66C58-E3D8-4490-AC75-DEF65AD38923}"/>
+    <hyperlink ref="C248" r:id="rId174" xr:uid="{B0E63A93-CE83-4004-924E-4CD4A576038F}"/>
+    <hyperlink ref="C249" r:id="rId175" xr:uid="{720AE4F0-6456-4B28-9400-B1134FD0944A}"/>
+    <hyperlink ref="C250" r:id="rId176" xr:uid="{AFF68C18-297D-4693-AC30-DFCA5C7942F7}"/>
+    <hyperlink ref="C252" r:id="rId177" xr:uid="{CF82DCDD-8086-4097-8513-CBD611B7084D}"/>
+    <hyperlink ref="C253" r:id="rId178" xr:uid="{95DAA79B-E338-485C-8CCC-8CE0439A75A5}"/>
+    <hyperlink ref="C254" r:id="rId179" xr:uid="{24F1050E-22C5-4DC9-9B5C-8087656F5DD4}"/>
+    <hyperlink ref="C255" r:id="rId180" xr:uid="{1175D431-461C-4303-A1C0-537EEB99E4B5}"/>
+    <hyperlink ref="C256" r:id="rId181" xr:uid="{67B0FFC9-D690-41E3-A5D1-4CE659B734B9}"/>
+    <hyperlink ref="C257" r:id="rId182" xr:uid="{112098E6-FB8E-4C6A-8BA3-8CE9DBD3F8A8}"/>
+    <hyperlink ref="C258" r:id="rId183" xr:uid="{5DD71B4C-52BD-4353-A062-2327991B2F35}"/>
+    <hyperlink ref="C259" r:id="rId184" xr:uid="{86F4C953-184D-4A20-B437-9F47CFECFC9D}"/>
+    <hyperlink ref="C260" r:id="rId185" xr:uid="{4F71BA32-866F-4718-9385-6F67B79D4870}"/>
+    <hyperlink ref="C261" r:id="rId186" xr:uid="{39CD2FB7-8639-4B5A-82E7-0E009B1621A5}"/>
+    <hyperlink ref="C262" r:id="rId187" xr:uid="{B98A8FF6-7A76-4F18-9358-31078AE94F9F}"/>
+    <hyperlink ref="B263" r:id="rId188" xr:uid="{DE96C102-1B62-4FE4-A6A7-B7A3EE98C8B9}"/>
+    <hyperlink ref="C263" r:id="rId189" xr:uid="{896C395F-298E-4509-9175-1901F37278F8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE4BE1E-D098-4EB7-9768-3C4DBF16DCB0}">
+  <dimension ref="C1:G134"/>
+  <sheetViews>
+    <sheetView topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:E134"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="119.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="4">
+        <v>45724.771736111114</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="7">
+        <v>45724.772939814815</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="9"/>
+    </row>
+    <row r="5" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="4">
+        <v>45724.777685185189</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="31">
+        <v>30509051400865</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="7">
+        <v>45724.783252314817</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="9"/>
+    </row>
+    <row r="7" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="4">
+        <v>45724.800636574073</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="7">
+        <v>45724.803206018521</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="4">
+        <v>45724.805752314816</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="31">
+        <v>20233360</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="7">
+        <v>45724.812673611108</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="9"/>
+    </row>
+    <row r="11" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="4">
+        <v>45725.53019675926</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="7">
+        <v>45726.039942129632</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="4">
+        <v>45726.04005787037</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+    </row>
+    <row r="14" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="7">
+        <v>45726.356793981482</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="8"/>
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="4">
+        <v>45726.357164351852</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="7">
+        <v>45726.466319444444</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="9"/>
+    </row>
+    <row r="17" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="4">
+        <v>45726.506782407407</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6"/>
+    </row>
+    <row r="18" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="7">
+        <v>45726.507210648146</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="9"/>
+    </row>
+    <row r="19" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="4">
+        <v>45727.02065972222</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="5"/>
+      <c r="G19" s="6"/>
+    </row>
+    <row r="20" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="7">
+        <v>45727.022858796299</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="9"/>
+    </row>
+    <row r="21" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="4">
+        <v>45727.029664351852</v>
+      </c>
+      <c r="D21" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="5"/>
+      <c r="G21" s="6"/>
+    </row>
+    <row r="22" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="7">
+        <v>45727.032870370371</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="30">
+        <v>20233360</v>
+      </c>
+      <c r="F22" s="8"/>
+      <c r="G22" s="9"/>
+    </row>
+    <row r="23" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="4">
+        <v>45727.033043981479</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="31">
+        <v>20233360</v>
+      </c>
+      <c r="F23" s="5"/>
+      <c r="G23" s="6"/>
+    </row>
+    <row r="24" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="7">
+        <v>45727.039386574077</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="9"/>
+    </row>
+    <row r="25" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="4">
+        <v>45727.051342592589</v>
+      </c>
+      <c r="D25" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" s="5"/>
+      <c r="G25" s="6"/>
+    </row>
+    <row r="26" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="7">
+        <v>45727.055520833332</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" s="8"/>
+      <c r="G26" s="9"/>
+    </row>
+    <row r="27" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="4">
+        <v>45727.348298611112</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" s="5"/>
+      <c r="G27" s="6"/>
+    </row>
+    <row r="28" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="7">
+        <v>45727.348761574074</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="F28" s="8"/>
+      <c r="G28" s="9"/>
+    </row>
+    <row r="29" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="4">
+        <v>45727.550428240742</v>
+      </c>
+      <c r="D29" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" s="5"/>
+      <c r="G29" s="6"/>
+    </row>
+    <row r="30" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="7">
+        <v>45730.132939814815</v>
+      </c>
+      <c r="D30" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" s="8"/>
+      <c r="G30" s="9"/>
+    </row>
+    <row r="31" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="4">
+        <v>45730.667627314811</v>
+      </c>
+      <c r="D31" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="F31" s="5"/>
+      <c r="G31" s="6"/>
+    </row>
+    <row r="32" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="7">
+        <v>45730.668043981481</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="F32" s="8"/>
+      <c r="G32" s="9"/>
+    </row>
+    <row r="33" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="4">
+        <v>45730.692094907405</v>
+      </c>
+      <c r="D33" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="F33" s="5"/>
+      <c r="G33" s="6"/>
+    </row>
+    <row r="34" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="7">
+        <v>45731.041458333333</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="F34" s="8"/>
+      <c r="G34" s="9"/>
+    </row>
+    <row r="35" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="4">
+        <v>45731.042604166665</v>
+      </c>
+      <c r="D35" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F35" s="5"/>
+      <c r="G35" s="6"/>
+    </row>
+    <row r="36" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C36" s="7">
+        <v>45731.383217592593</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="E36" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="F36" s="8"/>
+      <c r="G36" s="9"/>
+    </row>
+    <row r="37" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="4">
+        <v>45731.89230324074</v>
+      </c>
+      <c r="D37" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="E37" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="F37" s="5"/>
+      <c r="G37" s="6"/>
+    </row>
+    <row r="38" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="7">
+        <v>45731.892442129632</v>
+      </c>
+      <c r="D38" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="E38" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="F38" s="8"/>
+      <c r="G38" s="9"/>
+    </row>
+    <row r="39" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C39" s="4">
+        <v>45731.893680555557</v>
+      </c>
+      <c r="D39" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E39" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="F39" s="5"/>
+      <c r="G39" s="6"/>
+    </row>
+    <row r="40" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C40" s="7">
+        <v>45731.893842592595</v>
+      </c>
+      <c r="D40" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="E40" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="F40" s="8"/>
+      <c r="G40" s="9"/>
+    </row>
+    <row r="41" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="4">
+        <v>45731.895567129628</v>
+      </c>
+      <c r="D41" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="E41" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="F41" s="5"/>
+      <c r="G41" s="6"/>
+    </row>
+    <row r="42" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="7">
+        <v>45733.789525462962</v>
+      </c>
+      <c r="D42" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F42" s="8"/>
+      <c r="G42" s="9"/>
+    </row>
+    <row r="43" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C43" s="4">
+        <v>45733.795115740744</v>
+      </c>
+      <c r="D43" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="E43" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="F43" s="5"/>
+      <c r="G43" s="6"/>
+    </row>
+    <row r="44" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C44" s="7">
+        <v>45733.800370370373</v>
+      </c>
+      <c r="D44" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E44" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F44" s="8"/>
+      <c r="G44" s="9"/>
+    </row>
+    <row r="45" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C45" s="4">
+        <v>45733.805578703701</v>
+      </c>
+      <c r="D45" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="E45" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="F45" s="5"/>
+      <c r="G45" s="6"/>
+    </row>
+    <row r="46" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C46" s="7">
+        <v>45733.80641203704</v>
+      </c>
+      <c r="D46" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E46" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="F46" s="8"/>
+      <c r="G46" s="9"/>
+    </row>
+    <row r="47" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C47" s="4">
+        <v>45733.816261574073</v>
+      </c>
+      <c r="D47" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="E47" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="F47" s="5"/>
+      <c r="G47" s="6"/>
+    </row>
+    <row r="48" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C48" s="7">
+        <v>45735.574652777781</v>
+      </c>
+      <c r="D48" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="E48" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="F48" s="8"/>
+      <c r="G48" s="9"/>
+    </row>
+    <row r="49" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C49" s="4">
+        <v>45733.827337962961</v>
+      </c>
+      <c r="D49" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E49" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="F49" s="5"/>
+      <c r="G49" s="6"/>
+    </row>
+    <row r="50" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C50" s="7">
+        <v>45733.838587962964</v>
+      </c>
+      <c r="D50" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="E50" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="F50" s="8"/>
+      <c r="G50" s="9"/>
+    </row>
+    <row r="51" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C51" s="4">
+        <v>45733.851712962962</v>
+      </c>
+      <c r="D51" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E51" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="F51" s="5"/>
+      <c r="G51" s="6"/>
+    </row>
+    <row r="52" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C52" s="7">
+        <v>45733.881053240744</v>
+      </c>
+      <c r="D52" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="E52" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="F52" s="8"/>
+      <c r="G52" s="9"/>
+    </row>
+    <row r="53" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C53" s="4">
+        <v>45735.546041666668</v>
+      </c>
+      <c r="D53" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="E53" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="F53" s="5"/>
+      <c r="G53" s="6"/>
+    </row>
+    <row r="54" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C54" s="7">
+        <v>45733.974374999998</v>
+      </c>
+      <c r="D54" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="E54" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="F54" s="8"/>
+      <c r="G54" s="9"/>
+    </row>
+    <row r="55" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C55" s="4">
+        <v>45733.987372685187</v>
+      </c>
+      <c r="D55" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="E55" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="F55" s="5"/>
+      <c r="G55" s="6"/>
+    </row>
+    <row r="56" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C56" s="7">
+        <v>45733.991678240738</v>
+      </c>
+      <c r="D56" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="E56" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="F56" s="8"/>
+      <c r="G56" s="9"/>
+    </row>
+    <row r="57" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C57" s="4">
+        <v>45734.08734953704</v>
+      </c>
+      <c r="D57" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="E57" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="F57" s="5"/>
+      <c r="G57" s="6"/>
+    </row>
+    <row r="58" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C58" s="7">
+        <v>45734.128171296295</v>
+      </c>
+      <c r="D58" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="E58" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="F58" s="8"/>
+      <c r="G58" s="9"/>
+    </row>
+    <row r="59" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C59" s="4">
+        <v>45734.495439814818</v>
+      </c>
+      <c r="D59" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="E59" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="F59" s="5"/>
+      <c r="G59" s="6"/>
+    </row>
+    <row r="60" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C60" s="7">
+        <v>45734.552002314813</v>
+      </c>
+      <c r="D60" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="E60" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="F60" s="8"/>
+      <c r="G60" s="9"/>
+    </row>
+    <row r="61" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C61" s="4">
+        <v>45734.606840277775</v>
+      </c>
+      <c r="D61" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="E61" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="F61" s="5"/>
+      <c r="G61" s="6"/>
+    </row>
+    <row r="62" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C62" s="7">
+        <v>45734.612662037034</v>
+      </c>
+      <c r="D62" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="E62" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="F62" s="8"/>
+      <c r="G62" s="9"/>
+    </row>
+    <row r="63" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C63" s="4">
+        <v>45734.63653935185</v>
+      </c>
+      <c r="D63" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="E63" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="F63" s="5"/>
+      <c r="G63" s="6"/>
+    </row>
+    <row r="64" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C64" s="7">
+        <v>45734.719652777778</v>
+      </c>
+      <c r="D64" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="E64" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="F64" s="8"/>
+      <c r="G64" s="9"/>
+    </row>
+    <row r="65" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C65" s="4">
+        <v>45734.721446759257</v>
+      </c>
+      <c r="D65" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="E65" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="F65" s="5"/>
+      <c r="G65" s="6"/>
+    </row>
+    <row r="66" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C66" s="7">
+        <v>45734.725555555553</v>
+      </c>
+      <c r="D66" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="E66" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="F66" s="8"/>
+      <c r="G66" s="9"/>
+    </row>
+    <row r="67" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C67" s="4">
+        <v>45734.728935185187</v>
+      </c>
+      <c r="D67" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="E67" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="F67" s="5"/>
+      <c r="G67" s="6"/>
+    </row>
+    <row r="68" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C68" s="7">
+        <v>45734.863935185182</v>
+      </c>
+      <c r="D68" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="E68" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="F68" s="8"/>
+      <c r="G68" s="9"/>
+    </row>
+    <row r="69" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C69" s="4">
+        <v>45735.164502314816</v>
+      </c>
+      <c r="D69" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="E69" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="F69" s="5"/>
+      <c r="G69" s="6"/>
+    </row>
+    <row r="70" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C70" s="7">
+        <v>45735.229097222225</v>
+      </c>
+      <c r="D70" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="E70" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="F70" s="8"/>
+      <c r="G70" s="9"/>
+    </row>
+    <row r="71" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C71" s="4">
+        <v>45735.262106481481</v>
+      </c>
+      <c r="D71" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="E71" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="F71" s="5"/>
+      <c r="G71" s="6"/>
+    </row>
+    <row r="72" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C72" s="7">
+        <v>45735.341168981482</v>
+      </c>
+      <c r="D72" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="E72" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="F72" s="8"/>
+      <c r="G72" s="9"/>
+    </row>
+    <row r="73" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C73" s="4">
+        <v>45735.395312499997</v>
+      </c>
+      <c r="D73" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E73" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="F73" s="5"/>
+      <c r="G73" s="6"/>
+    </row>
+    <row r="74" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C74" s="7">
+        <v>45735.414930555555</v>
+      </c>
+      <c r="D74" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="E74" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="F74" s="8"/>
+      <c r="G74" s="9"/>
+    </row>
+    <row r="75" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C75" s="4">
+        <v>45735.517326388886</v>
+      </c>
+      <c r="D75" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="E75" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="F75" s="5"/>
+      <c r="G75" s="6"/>
+    </row>
+    <row r="76" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C76" s="7">
+        <v>45735.634039351855</v>
+      </c>
+      <c r="D76" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="E76" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="F76" s="8"/>
+      <c r="G76" s="9"/>
+    </row>
+    <row r="77" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C77" s="4">
+        <v>45735.653171296297</v>
+      </c>
+      <c r="D77" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="E77" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="F77" s="5"/>
+      <c r="G77" s="6"/>
+    </row>
+    <row r="78" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C78" s="7">
+        <v>45735.656875000001</v>
+      </c>
+      <c r="D78" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="E78" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="F78" s="8"/>
+      <c r="G78" s="9"/>
+    </row>
+    <row r="79" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C79" s="4">
+        <v>45735.669131944444</v>
+      </c>
+      <c r="D79" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="E79" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="F79" s="5"/>
+      <c r="G79" s="6"/>
+    </row>
+    <row r="80" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C80" s="7">
+        <v>45735.683749999997</v>
+      </c>
+      <c r="D80" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="E80" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="F80" s="8"/>
+      <c r="G80" s="9"/>
+    </row>
+    <row r="81" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C81" s="4">
+        <v>45735.722696759258</v>
+      </c>
+      <c r="D81" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="E81" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="F81" s="5"/>
+      <c r="G81" s="6"/>
+    </row>
+    <row r="82" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C82" s="7">
+        <v>45735.73709490741</v>
+      </c>
+      <c r="D82" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="E82" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="F82" s="8"/>
+      <c r="G82" s="9"/>
+    </row>
+    <row r="83" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C83" s="4">
+        <v>45735.791226851848</v>
+      </c>
+      <c r="D83" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="E83" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="F83" s="5"/>
+      <c r="G83" s="6"/>
+    </row>
+    <row r="84" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C84" s="7">
+        <v>45735.815532407411</v>
+      </c>
+      <c r="D84" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="E84" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="F84" s="8"/>
+      <c r="G84" s="9"/>
+    </row>
+    <row r="85" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C85" s="4">
+        <v>45735.83017361111</v>
+      </c>
+      <c r="D85" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="E85" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="F85" s="5"/>
+      <c r="G85" s="6"/>
+    </row>
+    <row r="86" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C86" s="7">
+        <v>45735.904293981483</v>
+      </c>
+      <c r="D86" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="E86" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="F86" s="8"/>
+      <c r="G86" s="9"/>
+    </row>
+    <row r="87" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C87" s="4">
+        <v>45735.916076388887</v>
+      </c>
+      <c r="D87" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="E87" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="F87" s="5"/>
+      <c r="G87" s="6"/>
+    </row>
+    <row r="88" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C88" s="7">
+        <v>45735.931064814817</v>
+      </c>
+      <c r="D88" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="E88" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="F88" s="8"/>
+      <c r="G88" s="9"/>
+    </row>
+    <row r="89" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C89" s="4">
+        <v>45735.954722222225</v>
+      </c>
+      <c r="D89" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="E89" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="F89" s="5"/>
+      <c r="G89" s="6"/>
+    </row>
+    <row r="90" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C90" s="7">
+        <v>45736.216805555552</v>
+      </c>
+      <c r="D90" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="E90" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="F90" s="8"/>
+      <c r="G90" s="9"/>
+    </row>
+    <row r="91" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C91" s="4">
+        <v>45736.221365740741</v>
+      </c>
+      <c r="D91" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="E91" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="F91" s="5"/>
+      <c r="G91" s="6"/>
+    </row>
+    <row r="92" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C92" s="7">
+        <v>45736.383368055554</v>
+      </c>
+      <c r="D92" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="E92" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="F92" s="8"/>
+      <c r="G92" s="9"/>
+    </row>
+    <row r="93" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C93" s="4">
+        <v>45736.435949074075</v>
+      </c>
+      <c r="D93" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="E93" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="F93" s="5"/>
+      <c r="G93" s="6"/>
+    </row>
+    <row r="94" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C94" s="7">
+        <v>45736.531006944446</v>
+      </c>
+      <c r="D94" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="E94" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="F94" s="8"/>
+      <c r="G94" s="9"/>
+    </row>
+    <row r="95" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C95" s="4">
+        <v>45736.532453703701</v>
+      </c>
+      <c r="D95" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="E95" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="F95" s="5"/>
+      <c r="G95" s="6"/>
+    </row>
+    <row r="96" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C96" s="7">
+        <v>45736.622372685182</v>
+      </c>
+      <c r="D96" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="E96" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="F96" s="8"/>
+      <c r="G96" s="9"/>
+    </row>
+    <row r="97" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C97" s="4">
+        <v>45736.630844907406</v>
+      </c>
+      <c r="D97" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="E97" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="F97" s="5"/>
+      <c r="G97" s="6"/>
+    </row>
+    <row r="98" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C98" s="7">
+        <v>45736.789652777778</v>
+      </c>
+      <c r="D98" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="E98" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="F98" s="8"/>
+      <c r="G98" s="9"/>
+    </row>
+    <row r="99" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C99" s="4">
+        <v>45736.954583333332</v>
+      </c>
+      <c r="D99" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="E99" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="F99" s="5"/>
+      <c r="G99" s="6"/>
+    </row>
+    <row r="100" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C100" s="7">
+        <v>45736.958553240744</v>
+      </c>
+      <c r="D100" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="E100" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="F100" s="8"/>
+      <c r="G100" s="9"/>
+    </row>
+    <row r="101" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C101" s="4">
+        <v>45736.958796296298</v>
+      </c>
+      <c r="D101" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="E101" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="F101" s="5"/>
+      <c r="G101" s="6"/>
+    </row>
+    <row r="102" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C102" s="7">
+        <v>45737.594444444447</v>
+      </c>
+      <c r="D102" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="E102" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="F102" s="8"/>
+      <c r="G102" s="9"/>
+    </row>
+    <row r="103" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C103" s="4">
+        <v>45737.594560185185</v>
+      </c>
+      <c r="D103" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="E103" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="F103" s="5"/>
+      <c r="G103" s="6"/>
+    </row>
+    <row r="104" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C104" s="7">
+        <v>45737.594675925924</v>
+      </c>
+      <c r="D104" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="E104" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="F104" s="8"/>
+      <c r="G104" s="9"/>
+    </row>
+    <row r="105" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C105" s="4">
+        <v>45737.625115740739</v>
+      </c>
+      <c r="D105" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="E105" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="F105" s="5"/>
+      <c r="G105" s="6"/>
+    </row>
+    <row r="106" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C106" s="7">
+        <v>45737.638344907406</v>
+      </c>
+      <c r="D106" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="E106" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="F106" s="8"/>
+      <c r="G106" s="9"/>
+    </row>
+    <row r="107" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C107" s="4">
+        <v>45737.638645833336</v>
+      </c>
+      <c r="D107" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="E107" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="F107" s="5"/>
+      <c r="G107" s="6"/>
+    </row>
+    <row r="108" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C108" s="7">
+        <v>45737.662002314813</v>
+      </c>
+      <c r="D108" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="E108" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="F108" s="8"/>
+      <c r="G108" s="9"/>
+    </row>
+    <row r="109" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C109" s="4">
+        <v>45737.693680555552</v>
+      </c>
+      <c r="D109" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="E109" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="F109" s="5"/>
+      <c r="G109" s="6"/>
+    </row>
+    <row r="110" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C110" s="7">
+        <v>45737.693831018521</v>
+      </c>
+      <c r="D110" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="E110" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="F110" s="8"/>
+      <c r="G110" s="9"/>
+    </row>
+    <row r="111" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C111" s="4">
+        <v>45737.7031712963</v>
+      </c>
+      <c r="D111" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="E111" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="F111" s="5"/>
+      <c r="G111" s="6"/>
+    </row>
+    <row r="112" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C112" s="7">
+        <v>45737.703530092593</v>
+      </c>
+      <c r="D112" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="E112" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="F112" s="8"/>
+      <c r="G112" s="9"/>
+    </row>
+    <row r="113" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C113" s="4">
+        <v>45737.87636574074</v>
+      </c>
+      <c r="D113" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="E113" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="F113" s="5"/>
+      <c r="G113" s="6"/>
+    </row>
+    <row r="114" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C114" s="7">
+        <v>45737.876574074071</v>
+      </c>
+      <c r="D114" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="E114" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="F114" s="8"/>
+      <c r="G114" s="9"/>
+    </row>
+    <row r="115" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C115" s="4">
+        <v>45737.987118055556</v>
+      </c>
+      <c r="D115" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="E115" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="F115" s="5"/>
+      <c r="G115" s="6"/>
+    </row>
+    <row r="116" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C116" s="7">
+        <v>45738.049212962964</v>
+      </c>
+      <c r="D116" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="E116" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="F116" s="8"/>
+      <c r="G116" s="9"/>
+    </row>
+    <row r="117" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C117" s="4">
+        <v>45738.637048611112</v>
+      </c>
+      <c r="D117" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="E117" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="F117" s="5"/>
+      <c r="G117" s="6"/>
+    </row>
+    <row r="118" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C118" s="7">
+        <v>45738.637326388889</v>
+      </c>
+      <c r="D118" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="E118" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="F118" s="8"/>
+      <c r="G118" s="9"/>
+    </row>
+    <row r="119" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C119" s="4">
+        <v>45738.740254629629</v>
+      </c>
+      <c r="D119" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="E119" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="F119" s="5"/>
+      <c r="G119" s="6"/>
+    </row>
+    <row r="120" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C120" s="7">
+        <v>45738.740439814814</v>
+      </c>
+      <c r="D120" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="E120" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="F120" s="8"/>
+      <c r="G120" s="9"/>
+    </row>
+    <row r="121" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C121" s="4">
+        <v>45738.741099537037</v>
+      </c>
+      <c r="D121" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="E121" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="F121" s="5"/>
+      <c r="G121" s="6"/>
+    </row>
+    <row r="122" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C122" s="7">
+        <v>45739.096574074072</v>
+      </c>
+      <c r="D122" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="E122" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="F122" s="8"/>
+      <c r="G122" s="9"/>
+    </row>
+    <row r="123" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C123" s="4">
+        <v>45739.616539351853</v>
+      </c>
+      <c r="D123" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="E123" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="F123" s="5"/>
+      <c r="G123" s="6"/>
+    </row>
+    <row r="124" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C124" s="7">
+        <v>45740.519872685189</v>
+      </c>
+      <c r="D124" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="E124" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="F124" s="8"/>
+      <c r="G124" s="9"/>
+    </row>
+    <row r="125" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C125" s="4">
+        <v>45742.76363425926</v>
+      </c>
+      <c r="D125" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="E125" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="F125" s="5"/>
+      <c r="G125" s="6"/>
+    </row>
+    <row r="126" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C126" s="7">
+        <v>45743.680300925924</v>
+      </c>
+      <c r="D126" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="E126" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="F126" s="8"/>
+      <c r="G126" s="9"/>
+    </row>
+    <row r="127" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C127" s="4">
+        <v>45746.572465277779</v>
+      </c>
+      <c r="D127" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="E127" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="F127" s="5"/>
+      <c r="G127" s="6"/>
+    </row>
+    <row r="128" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C128" s="7">
+        <v>45754.547407407408</v>
+      </c>
+      <c r="D128" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="E128" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="F128" s="8"/>
+      <c r="G128" s="9"/>
+    </row>
+    <row r="129" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C129" s="4">
+        <v>45756.423807870371</v>
+      </c>
+      <c r="D129" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="E129" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="F129" s="5"/>
+      <c r="G129" s="6"/>
+    </row>
+    <row r="130" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C130" s="7">
+        <v>45756.662766203706</v>
+      </c>
+      <c r="D130" s="29" t="s">
+        <v>170</v>
+      </c>
+      <c r="E130" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="F130" s="8"/>
+      <c r="G130" s="9"/>
+    </row>
+    <row r="131" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C131" s="4">
+        <v>45756.682824074072</v>
+      </c>
+      <c r="D131" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="E131" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="F131" s="5"/>
+      <c r="G131" s="6"/>
+    </row>
+    <row r="132" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C132" s="7">
+        <v>45756.682974537034</v>
+      </c>
+      <c r="D132" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="E132" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="F132" s="8"/>
+      <c r="G132" s="9"/>
+    </row>
+    <row r="133" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C133" s="4">
+        <v>45757.531770833331</v>
+      </c>
+      <c r="D133" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="E133" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="F133" s="5"/>
+      <c r="G133" s="6"/>
+    </row>
+    <row r="134" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C134" s="10">
+        <v>45759.652187500003</v>
+      </c>
+      <c r="D134" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="E134" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="F134" s="11"/>
+      <c r="G134" s="12"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{F1E9BD74-B617-42B1-893F-CF8BF982BFAD}"/>
+    <hyperlink ref="E6" r:id="rId2" xr:uid="{4B239A6E-0869-4E0A-9FA4-D4C809244E0C}"/>
+    <hyperlink ref="E10" r:id="rId3" xr:uid="{6213795D-670C-49E9-8A54-F7D9F9CB3040}"/>
+    <hyperlink ref="E12" r:id="rId4" xr:uid="{D274EC45-DA75-484E-AD31-CC3E74A3B301}"/>
+    <hyperlink ref="E13" r:id="rId5" xr:uid="{B23F349C-30F9-4F85-B5C4-537DBEBEC7CD}"/>
+    <hyperlink ref="E19" r:id="rId6" xr:uid="{4EA4265E-9D15-4F2A-BD13-58AFDB3454D7}"/>
+    <hyperlink ref="E21" r:id="rId7" xr:uid="{14E48C6B-F3FF-402D-8F55-825A94B71745}"/>
+    <hyperlink ref="E25" r:id="rId8" xr:uid="{664A1C0F-756D-412D-B2F6-9BFDE325DA08}"/>
+    <hyperlink ref="E26" r:id="rId9" xr:uid="{E208BCD5-AE43-4520-AB2E-BB14445E511E}"/>
+    <hyperlink ref="E27" r:id="rId10" xr:uid="{32FFA529-C98F-4404-9B26-B7344EB9ECA3}"/>
+    <hyperlink ref="E28" r:id="rId11" xr:uid="{6A058655-8EEC-4394-94D4-171A5244D033}"/>
+    <hyperlink ref="E29" r:id="rId12" xr:uid="{F3A8A684-8CAD-496F-A1BA-7D7F45FBFBDF}"/>
+    <hyperlink ref="E30" r:id="rId13" xr:uid="{63A6E579-990B-4C8F-A6D2-2E091F8B75FF}"/>
+    <hyperlink ref="E31" r:id="rId14" xr:uid="{C3F13DA3-EFCB-44DF-B441-8E829DB1359A}"/>
+    <hyperlink ref="E32" r:id="rId15" xr:uid="{CFCFF2AB-3C69-4729-8402-D77BF49F0D79}"/>
+    <hyperlink ref="E33" r:id="rId16" xr:uid="{B90919A0-2D03-41D1-98D1-151572BCFB5D}"/>
+    <hyperlink ref="E36" r:id="rId17" xr:uid="{F062E9C5-86C1-4CF1-8D4E-576A74443984}"/>
+    <hyperlink ref="E37" r:id="rId18" xr:uid="{1E5FA45C-7BC0-4F57-9ABD-CAA728EEBCBC}"/>
+    <hyperlink ref="E38" r:id="rId19" xr:uid="{8AE69837-736F-4218-9137-7705C4F2FC46}"/>
+    <hyperlink ref="E39" r:id="rId20" xr:uid="{D8F7CA9B-4F0E-4FBC-A5BE-BD117CFEF273}"/>
+    <hyperlink ref="E40" r:id="rId21" xr:uid="{E2A930C9-1408-4475-8A22-28E1282CD8FD}"/>
+    <hyperlink ref="E43" r:id="rId22" xr:uid="{19C58405-5551-4842-85E5-2F57FE08ABE8}"/>
+    <hyperlink ref="E45" r:id="rId23" xr:uid="{6A3B2EEE-A8F0-4878-ADEF-FC15B66B05B0}"/>
+    <hyperlink ref="E47" r:id="rId24" xr:uid="{50DBB9DF-1EB5-4B4C-9B72-89EFE8906780}"/>
+    <hyperlink ref="E48" r:id="rId25" xr:uid="{20EA74E2-1BD2-44C7-B609-607A22CEF453}"/>
+    <hyperlink ref="E50" r:id="rId26" xr:uid="{4C6A92F7-673F-4835-A0E2-4E1F2399C446}"/>
+    <hyperlink ref="E51" r:id="rId27" xr:uid="{9CAA46B0-C10E-48A3-B97C-F31731DCAF90}"/>
+    <hyperlink ref="E53" r:id="rId28" xr:uid="{46059E33-73CF-47F9-95E0-9610F14B2402}"/>
+    <hyperlink ref="E54" r:id="rId29" xr:uid="{648AFC1B-22F5-43A8-AB30-74CA08637BDE}"/>
+    <hyperlink ref="E55" r:id="rId30" xr:uid="{C5548410-26B3-4999-9F46-A32AE15BB71E}"/>
+    <hyperlink ref="E56" r:id="rId31" xr:uid="{B2DB7B47-AC8B-4C88-98B3-4FCFCB68FE51}"/>
+    <hyperlink ref="E58" r:id="rId32" xr:uid="{2D0B801E-C6BB-4724-A5CF-7B21413C86F5}"/>
+    <hyperlink ref="E60" r:id="rId33" xr:uid="{40E5DCBB-1316-4F98-9128-A9E0915870EA}"/>
+    <hyperlink ref="E61" r:id="rId34" xr:uid="{CB6FDEA4-84F5-440D-899A-49BFD4EFAEDC}"/>
+    <hyperlink ref="E63" r:id="rId35" xr:uid="{5B6BFAB9-3718-4A83-AF57-A1EA51792951}"/>
+    <hyperlink ref="E64" r:id="rId36" xr:uid="{A1D837A8-90EB-4CC0-B2D0-BF705DF67A01}"/>
+    <hyperlink ref="E65" r:id="rId37" xr:uid="{DD1FF8CF-D802-4BCD-A1C4-A5C87777B40B}"/>
+    <hyperlink ref="E66" r:id="rId38" xr:uid="{B4C5687C-5C33-47D0-90EA-BDB13F2FC0F5}"/>
+    <hyperlink ref="E67" r:id="rId39" xr:uid="{50563910-D00C-49EF-A930-5E17F4EC7A1F}"/>
+    <hyperlink ref="E68" r:id="rId40" xr:uid="{DF8FDDDF-2292-4EA3-9A44-C0F77BE4B6CE}"/>
+    <hyperlink ref="E71" r:id="rId41" xr:uid="{6AF62F41-F9EB-4A72-A20C-32E0447D919A}"/>
+    <hyperlink ref="E72" r:id="rId42" xr:uid="{62042588-2E73-48F8-B4FA-9D34893588DA}"/>
+    <hyperlink ref="E73" r:id="rId43" xr:uid="{6EA8A875-106E-489F-A625-C6459C4088E0}"/>
+    <hyperlink ref="E74" r:id="rId44" xr:uid="{89670EDD-B9B1-4CF9-86ED-E71B209FD907}"/>
+    <hyperlink ref="E75" r:id="rId45" xr:uid="{3C33C2E5-3D23-48D1-8949-26274195583D}"/>
+    <hyperlink ref="E77" r:id="rId46" display="https://rahma5555.github.io/roro00/" xr:uid="{D308997D-C6BE-4A15-960A-AC32D4D94848}"/>
+    <hyperlink ref="E78" r:id="rId47" xr:uid="{E9985539-FA90-4985-8574-FE7ED2E3556D}"/>
+    <hyperlink ref="E79" r:id="rId48" xr:uid="{2B700A39-1AB9-472A-ADC3-CB897401956D}"/>
+    <hyperlink ref="E80" r:id="rId49" xr:uid="{C10DE254-DEED-4A9C-9DC4-25AD39B15F08}"/>
+    <hyperlink ref="E81" r:id="rId50" xr:uid="{97C2A39B-7FE1-4995-AF55-DA3F019FF0C1}"/>
+    <hyperlink ref="E82" r:id="rId51" xr:uid="{74401B6D-40C2-488F-BEEE-90D836E92002}"/>
+    <hyperlink ref="E83" r:id="rId52" xr:uid="{670F00C2-4564-4667-AFA6-9B76ED94B65D}"/>
+    <hyperlink ref="E87" r:id="rId53" xr:uid="{F0A1C0A4-7449-4215-B2CD-945640E4C879}"/>
+    <hyperlink ref="E88" r:id="rId54" xr:uid="{5B7A631F-0DAC-4353-AC1B-5DD79D8574EE}"/>
+    <hyperlink ref="E89" r:id="rId55" xr:uid="{145D794B-E753-4FDD-A251-698EA8827CE4}"/>
+    <hyperlink ref="E90" r:id="rId56" xr:uid="{A1129247-88EB-4897-9A51-377D1A58B799}"/>
+    <hyperlink ref="E91" r:id="rId57" display="https://loloah20.githup.io/sva20/" xr:uid="{F5C4C357-E455-49F8-A05E-024CBA9FFC50}"/>
+    <hyperlink ref="E93" r:id="rId58" xr:uid="{1FEA772F-2D05-4C8C-A80C-67468E6451A3}"/>
+    <hyperlink ref="E94" r:id="rId59" xr:uid="{9D40D9E0-DBDC-46BF-AE8D-5B3FF2EC1B79}"/>
+    <hyperlink ref="E95" r:id="rId60" xr:uid="{021C3CA8-B193-468F-8CD0-9D11B3EA3CAB}"/>
+    <hyperlink ref="E97" r:id="rId61" xr:uid="{FBE4702E-B39B-41B4-BB14-693515EE2E76}"/>
+    <hyperlink ref="E98" r:id="rId62" display="https://abdullahmahmoud20234326.github.io/myweb/" xr:uid="{66D14907-BA0F-4A07-B706-EFCB28692EE2}"/>
+    <hyperlink ref="E99" r:id="rId63" xr:uid="{8B1B00DD-A7F4-42FF-8989-96F30E34C0B8}"/>
+    <hyperlink ref="E100" r:id="rId64" xr:uid="{339F7C50-3890-49AA-AB27-EA4C121B8CD4}"/>
+    <hyperlink ref="E101" r:id="rId65" xr:uid="{C222D95B-471A-4D13-81D8-09A739A2F2A3}"/>
+    <hyperlink ref="E102" r:id="rId66" xr:uid="{7D4CF153-DD0C-4BA1-8DC5-E7FA6AD2273E}"/>
+    <hyperlink ref="E103" r:id="rId67" xr:uid="{B0A3FB84-3C92-44A7-A9B2-6A7E6CF1234B}"/>
+    <hyperlink ref="E104" r:id="rId68" xr:uid="{602AD707-7D4D-495A-AF4E-2F6EAD107592}"/>
+    <hyperlink ref="E105" r:id="rId69" display="https://basant1512006.github.io/basant-walid/" xr:uid="{0C664C73-B17A-4502-B968-94E167DF42C0}"/>
+    <hyperlink ref="E106" r:id="rId70" xr:uid="{D215A287-EE72-4ABF-8035-FC46456A6ED4}"/>
+    <hyperlink ref="E107" r:id="rId71" xr:uid="{62A9721D-E74F-4891-98CD-1D8E906D9EB2}"/>
+    <hyperlink ref="E108" r:id="rId72" xr:uid="{38CCB2F7-8AFE-4C61-AF6C-269C7E5A5671}"/>
+    <hyperlink ref="E110" r:id="rId73" display="https://basant1512006.github.io/Rofida-gehad/" xr:uid="{783795E7-4D3B-475C-AD9D-4F36A7A6D9E8}"/>
+    <hyperlink ref="E111" r:id="rId74" xr:uid="{EFF439D5-B8C8-4F1E-BCCD-B4DAB0645D17}"/>
+    <hyperlink ref="E112" r:id="rId75" xr:uid="{E07D9E32-0374-4D2C-AB3F-4E1BB92C0473}"/>
+    <hyperlink ref="E113" r:id="rId76" xr:uid="{FC306888-5930-4017-81C3-EEEF3676B098}"/>
+    <hyperlink ref="E114" r:id="rId77" xr:uid="{43EAD1E0-0D89-487A-8426-7465F7CFC9C9}"/>
+    <hyperlink ref="E115" r:id="rId78" xr:uid="{434E66F2-4693-4FCD-B37F-54B73EA6503D}"/>
+    <hyperlink ref="E116" r:id="rId79" xr:uid="{6C1BFD19-2C91-4586-9D27-2E66CAB7D18C}"/>
+    <hyperlink ref="E117" r:id="rId80" xr:uid="{C92E710E-B025-4F7D-AFAA-943AFAAB60E0}"/>
+    <hyperlink ref="E118" r:id="rId81" xr:uid="{E466499E-9B3A-4A01-ACFB-D522B3316A1F}"/>
+    <hyperlink ref="E119" r:id="rId82" xr:uid="{5B1561AD-7AB7-4AA5-B762-FFA1D317E42F}"/>
+    <hyperlink ref="E120" r:id="rId83" xr:uid="{E2772DAA-486C-4C1D-B0C1-12DE0BB3DB26}"/>
+    <hyperlink ref="E121" r:id="rId84" xr:uid="{FCF797AC-428A-41F2-B568-CE39534F325B}"/>
+    <hyperlink ref="E122" r:id="rId85" xr:uid="{953FDC00-3AB0-45CE-955B-FC4FB1CB2771}"/>
+    <hyperlink ref="E124" r:id="rId86" xr:uid="{CD72FD9F-0C9C-44C5-A338-C8C387B9756D}"/>
+    <hyperlink ref="E125" r:id="rId87" xr:uid="{FEA3DBF3-7B45-49EB-A734-99505210C4B8}"/>
+    <hyperlink ref="E126" r:id="rId88" xr:uid="{C4857A75-C4FF-40E1-BF21-2A6E09555771}"/>
+    <hyperlink ref="E127" r:id="rId89" xr:uid="{D592619F-CB5F-4EFD-A5D3-A3ACA24F0DF5}"/>
+    <hyperlink ref="E128" r:id="rId90" xr:uid="{33177A24-E441-490F-96D9-D3D890FC485B}"/>
+    <hyperlink ref="E129" r:id="rId91" xr:uid="{7C6B22DD-7F00-4ACC-9DC0-D7861FC7686C}"/>
+    <hyperlink ref="E130" r:id="rId92" xr:uid="{D71395D0-1F33-4D5C-B03F-72791AD93B6F}"/>
+    <hyperlink ref="E131" r:id="rId93" xr:uid="{DE976379-35BF-458D-84FB-F1C769FEE336}"/>
+    <hyperlink ref="E132" r:id="rId94" xr:uid="{D87DD31F-E02B-44C1-93D6-F47AA5695D30}"/>
+    <hyperlink ref="E133" r:id="rId95" xr:uid="{1A58D559-3D9E-4510-B73A-0CB3EDFDBEB9}"/>
+    <hyperlink ref="E134" r:id="rId96" xr:uid="{6C9F5C82-30F9-4BDD-9EA2-2E7CFA0612D1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Record 14-04-2025 05:36
</commit_message>
<xml_diff>
--- a/Records.xlsx
+++ b/Records.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moh_zakria\Desktop\Students URLs\MyWeRepo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zicooo82/Desktop/معهد الوادي/MyWeRepo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61BEBCCD-E140-416C-96A0-339230CEF341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3330D30-A684-5742-9CE6-0ECC146A452F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="18000" windowHeight="9360" xr2:uid="{AE619845-176D-4C93-91F5-F1442B84480E}"/>
+    <workbookView xWindow="3460" yWindow="3460" windowWidth="18000" windowHeight="9360" xr2:uid="{AE619845-176D-4C93-91F5-F1442B84480E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="187">
   <si>
     <t>Timestamp</t>
   </si>
@@ -572,6 +572,24 @@
   </si>
   <si>
     <t>aw20230244@sva.edu.eg</t>
+  </si>
+  <si>
+    <t>me20233253@sva.edu.eg</t>
+  </si>
+  <si>
+    <t>https://mariam2005856.github.io/mariam_essam/</t>
+  </si>
+  <si>
+    <t>https://rehabezzat122.github.io/first-web-page/</t>
+  </si>
+  <si>
+    <t>re20231348@sva.edu.eg</t>
+  </si>
+  <si>
+    <t>https://eman2005820.github.io/mypage./</t>
+  </si>
+  <si>
+    <t>ea20230350@sva.edu.eg</t>
   </si>
 </sst>
 </file>
@@ -1025,9 +1043,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1065,7 +1083,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1171,7 +1189,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1313,7 +1331,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1321,22 +1339,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97601210-06D1-436F-9FFC-E5C230996E4C}">
-  <dimension ref="A1:E264"/>
+  <dimension ref="A1:E267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A261" workbookViewId="0">
-      <selection activeCell="B270" sqref="B270"/>
+    <sheetView tabSelected="1" topLeftCell="B261" workbookViewId="0">
+      <selection activeCell="B267" sqref="B267"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="119.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="119.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1353,7 +1371,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>45724.771736111114</v>
       </c>
@@ -1366,7 +1384,7 @@
       <c r="D2" s="5"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>45724.772939814815</v>
       </c>
@@ -1379,7 +1397,7 @@
       <c r="D3" s="8"/>
       <c r="E3" s="9"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>45724.777685185189</v>
       </c>
@@ -1392,7 +1410,7 @@
       <c r="D4" s="5"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>45724.783252314817</v>
       </c>
@@ -1405,7 +1423,7 @@
       <c r="D5" s="8"/>
       <c r="E5" s="9"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>45724.800636574073</v>
       </c>
@@ -1418,7 +1436,7 @@
       <c r="D6" s="5"/>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>45724.803206018521</v>
       </c>
@@ -1431,7 +1449,7 @@
       <c r="D7" s="8"/>
       <c r="E7" s="9"/>
     </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>45724.805752314816</v>
       </c>
@@ -1444,7 +1462,7 @@
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>45724.812673611108</v>
       </c>
@@ -1457,7 +1475,7 @@
       <c r="D9" s="8"/>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>45725.53019675926</v>
       </c>
@@ -1470,7 +1488,7 @@
       <c r="D10" s="5"/>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>45726.039942129632</v>
       </c>
@@ -1483,7 +1501,7 @@
       <c r="D11" s="8"/>
       <c r="E11" s="9"/>
     </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>45726.04005787037</v>
       </c>
@@ -1496,7 +1514,7 @@
       <c r="D12" s="5"/>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>45726.356793981482</v>
       </c>
@@ -1509,7 +1527,7 @@
       <c r="D13" s="8"/>
       <c r="E13" s="9"/>
     </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>45726.357164351852</v>
       </c>
@@ -1522,7 +1540,7 @@
       <c r="D14" s="5"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>45726.466319444444</v>
       </c>
@@ -1535,7 +1553,7 @@
       <c r="D15" s="8"/>
       <c r="E15" s="9"/>
     </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>45726.506782407407</v>
       </c>
@@ -1548,7 +1566,7 @@
       <c r="D16" s="5"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>45726.507210648146</v>
       </c>
@@ -1561,7 +1579,7 @@
       <c r="D17" s="8"/>
       <c r="E17" s="9"/>
     </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>45727.02065972222</v>
       </c>
@@ -1574,7 +1592,7 @@
       <c r="D18" s="5"/>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>45727.022858796299</v>
       </c>
@@ -1585,7 +1603,7 @@
       <c r="D19" s="8"/>
       <c r="E19" s="9"/>
     </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>45727.029664351852</v>
       </c>
@@ -1598,7 +1616,7 @@
       <c r="D20" s="5"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>45727.032870370371</v>
       </c>
@@ -1611,7 +1629,7 @@
       <c r="D21" s="8"/>
       <c r="E21" s="9"/>
     </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>45727.033043981479</v>
       </c>
@@ -1624,7 +1642,7 @@
       <c r="D22" s="5"/>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>45727.039386574077</v>
       </c>
@@ -1637,7 +1655,7 @@
       <c r="D23" s="8"/>
       <c r="E23" s="9"/>
     </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>45727.051342592589</v>
       </c>
@@ -1650,7 +1668,7 @@
       <c r="D24" s="5"/>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>45727.055520833332</v>
       </c>
@@ -1663,7 +1681,7 @@
       <c r="D25" s="8"/>
       <c r="E25" s="9"/>
     </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>45727.348298611112</v>
       </c>
@@ -1676,7 +1694,7 @@
       <c r="D26" s="5"/>
       <c r="E26" s="6"/>
     </row>
-    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>45727.348761574074</v>
       </c>
@@ -1689,7 +1707,7 @@
       <c r="D27" s="8"/>
       <c r="E27" s="9"/>
     </row>
-    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>45727.550428240742</v>
       </c>
@@ -1702,7 +1720,7 @@
       <c r="D28" s="5"/>
       <c r="E28" s="6"/>
     </row>
-    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>45730.132939814815</v>
       </c>
@@ -1715,7 +1733,7 @@
       <c r="D29" s="8"/>
       <c r="E29" s="9"/>
     </row>
-    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>45730.667627314811</v>
       </c>
@@ -1728,7 +1746,7 @@
       <c r="D30" s="5"/>
       <c r="E30" s="6"/>
     </row>
-    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>45730.668043981481</v>
       </c>
@@ -1741,7 +1759,7 @@
       <c r="D31" s="8"/>
       <c r="E31" s="9"/>
     </row>
-    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>45730.692094907405</v>
       </c>
@@ -1754,7 +1772,7 @@
       <c r="D32" s="5"/>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>45731.041458333333</v>
       </c>
@@ -1767,7 +1785,7 @@
       <c r="D33" s="8"/>
       <c r="E33" s="9"/>
     </row>
-    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>45731.042604166665</v>
       </c>
@@ -1780,7 +1798,7 @@
       <c r="D34" s="5"/>
       <c r="E34" s="6"/>
     </row>
-    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>45731.383217592593</v>
       </c>
@@ -1793,7 +1811,7 @@
       <c r="D35" s="8"/>
       <c r="E35" s="9"/>
     </row>
-    <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>45731.89230324074</v>
       </c>
@@ -1806,7 +1824,7 @@
       <c r="D36" s="5"/>
       <c r="E36" s="6"/>
     </row>
-    <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>45731.892442129632</v>
       </c>
@@ -1819,7 +1837,7 @@
       <c r="D37" s="8"/>
       <c r="E37" s="9"/>
     </row>
-    <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>45731.893680555557</v>
       </c>
@@ -1832,7 +1850,7 @@
       <c r="D38" s="5"/>
       <c r="E38" s="6"/>
     </row>
-    <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>45731.893842592595</v>
       </c>
@@ -1845,7 +1863,7 @@
       <c r="D39" s="8"/>
       <c r="E39" s="9"/>
     </row>
-    <row r="40" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>45731.895567129628</v>
       </c>
@@ -1858,7 +1876,7 @@
       <c r="D40" s="5"/>
       <c r="E40" s="6"/>
     </row>
-    <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>45733.789525462962</v>
       </c>
@@ -1871,7 +1889,7 @@
       <c r="D41" s="8"/>
       <c r="E41" s="9"/>
     </row>
-    <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>45733.795115740744</v>
       </c>
@@ -1884,7 +1902,7 @@
       <c r="D42" s="5"/>
       <c r="E42" s="6"/>
     </row>
-    <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>45733.800370370373</v>
       </c>
@@ -1897,7 +1915,7 @@
       <c r="D43" s="8"/>
       <c r="E43" s="9"/>
     </row>
-    <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>45733.805578703701</v>
       </c>
@@ -1910,7 +1928,7 @@
       <c r="D44" s="5"/>
       <c r="E44" s="6"/>
     </row>
-    <row r="45" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <v>45733.80641203704</v>
       </c>
@@ -1923,7 +1941,7 @@
       <c r="D45" s="8"/>
       <c r="E45" s="9"/>
     </row>
-    <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>45733.816261574073</v>
       </c>
@@ -1936,7 +1954,7 @@
       <c r="D46" s="5"/>
       <c r="E46" s="6"/>
     </row>
-    <row r="47" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>45735.574652777781</v>
       </c>
@@ -1949,7 +1967,7 @@
       <c r="D47" s="8"/>
       <c r="E47" s="9"/>
     </row>
-    <row r="48" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>45733.827337962961</v>
       </c>
@@ -1962,7 +1980,7 @@
       <c r="D48" s="5"/>
       <c r="E48" s="6"/>
     </row>
-    <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>45733.838587962964</v>
       </c>
@@ -1975,7 +1993,7 @@
       <c r="D49" s="8"/>
       <c r="E49" s="9"/>
     </row>
-    <row r="50" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>45733.851712962962</v>
       </c>
@@ -1988,7 +2006,7 @@
       <c r="D50" s="5"/>
       <c r="E50" s="6"/>
     </row>
-    <row r="51" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>45733.881053240744</v>
       </c>
@@ -2001,7 +2019,7 @@
       <c r="D51" s="8"/>
       <c r="E51" s="9"/>
     </row>
-    <row r="52" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>45735.546041666668</v>
       </c>
@@ -2014,7 +2032,7 @@
       <c r="D52" s="5"/>
       <c r="E52" s="6"/>
     </row>
-    <row r="53" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
         <v>45733.974374999998</v>
       </c>
@@ -2027,7 +2045,7 @@
       <c r="D53" s="8"/>
       <c r="E53" s="9"/>
     </row>
-    <row r="54" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>45733.987372685187</v>
       </c>
@@ -2040,7 +2058,7 @@
       <c r="D54" s="5"/>
       <c r="E54" s="6"/>
     </row>
-    <row r="55" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <v>45733.991678240738</v>
       </c>
@@ -2053,7 +2071,7 @@
       <c r="D55" s="8"/>
       <c r="E55" s="9"/>
     </row>
-    <row r="56" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>45734.08734953704</v>
       </c>
@@ -2066,7 +2084,7 @@
       <c r="D56" s="5"/>
       <c r="E56" s="6"/>
     </row>
-    <row r="57" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
         <v>45734.128171296295</v>
       </c>
@@ -2079,7 +2097,7 @@
       <c r="D57" s="8"/>
       <c r="E57" s="9"/>
     </row>
-    <row r="58" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>45734.495439814818</v>
       </c>
@@ -2092,7 +2110,7 @@
       <c r="D58" s="5"/>
       <c r="E58" s="6"/>
     </row>
-    <row r="59" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
         <v>45734.552002314813</v>
       </c>
@@ -2105,7 +2123,7 @@
       <c r="D59" s="8"/>
       <c r="E59" s="9"/>
     </row>
-    <row r="60" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>45734.606840277775</v>
       </c>
@@ -2118,7 +2136,7 @@
       <c r="D60" s="5"/>
       <c r="E60" s="6"/>
     </row>
-    <row r="61" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7">
         <v>45734.612662037034</v>
       </c>
@@ -2131,7 +2149,7 @@
       <c r="D61" s="8"/>
       <c r="E61" s="9"/>
     </row>
-    <row r="62" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>45734.63653935185</v>
       </c>
@@ -2144,7 +2162,7 @@
       <c r="D62" s="5"/>
       <c r="E62" s="6"/>
     </row>
-    <row r="63" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
         <v>45734.719652777778</v>
       </c>
@@ -2157,7 +2175,7 @@
       <c r="D63" s="8"/>
       <c r="E63" s="9"/>
     </row>
-    <row r="64" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>45734.721446759257</v>
       </c>
@@ -2170,7 +2188,7 @@
       <c r="D64" s="5"/>
       <c r="E64" s="6"/>
     </row>
-    <row r="65" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7">
         <v>45734.725555555553</v>
       </c>
@@ -2183,7 +2201,7 @@
       <c r="D65" s="8"/>
       <c r="E65" s="9"/>
     </row>
-    <row r="66" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>45734.728935185187</v>
       </c>
@@ -2196,7 +2214,7 @@
       <c r="D66" s="5"/>
       <c r="E66" s="6"/>
     </row>
-    <row r="67" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <v>45734.863935185182</v>
       </c>
@@ -2209,7 +2227,7 @@
       <c r="D67" s="8"/>
       <c r="E67" s="9"/>
     </row>
-    <row r="68" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>45735.164502314816</v>
       </c>
@@ -2222,7 +2240,7 @@
       <c r="D68" s="5"/>
       <c r="E68" s="6"/>
     </row>
-    <row r="69" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="7">
         <v>45735.229097222225</v>
       </c>
@@ -2235,7 +2253,7 @@
       <c r="D69" s="8"/>
       <c r="E69" s="9"/>
     </row>
-    <row r="70" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>45735.262106481481</v>
       </c>
@@ -2248,7 +2266,7 @@
       <c r="D70" s="5"/>
       <c r="E70" s="6"/>
     </row>
-    <row r="71" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A71" s="7">
         <v>45735.341168981482</v>
       </c>
@@ -2261,7 +2279,7 @@
       <c r="D71" s="8"/>
       <c r="E71" s="9"/>
     </row>
-    <row r="72" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>45735.395312499997</v>
       </c>
@@ -2274,7 +2292,7 @@
       <c r="D72" s="5"/>
       <c r="E72" s="6"/>
     </row>
-    <row r="73" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="7">
         <v>45735.414930555555</v>
       </c>
@@ -2287,7 +2305,7 @@
       <c r="D73" s="8"/>
       <c r="E73" s="9"/>
     </row>
-    <row r="74" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>45735.517326388886</v>
       </c>
@@ -2300,7 +2318,7 @@
       <c r="D74" s="5"/>
       <c r="E74" s="6"/>
     </row>
-    <row r="75" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="7">
         <v>45735.634039351855</v>
       </c>
@@ -2313,7 +2331,7 @@
       <c r="D75" s="8"/>
       <c r="E75" s="9"/>
     </row>
-    <row r="76" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>45735.653171296297</v>
       </c>
@@ -2326,7 +2344,7 @@
       <c r="D76" s="5"/>
       <c r="E76" s="6"/>
     </row>
-    <row r="77" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="7">
         <v>45735.656875000001</v>
       </c>
@@ -2339,7 +2357,7 @@
       <c r="D77" s="8"/>
       <c r="E77" s="9"/>
     </row>
-    <row r="78" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>45735.669131944444</v>
       </c>
@@ -2352,7 +2370,7 @@
       <c r="D78" s="5"/>
       <c r="E78" s="6"/>
     </row>
-    <row r="79" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="7">
         <v>45735.683749999997</v>
       </c>
@@ -2365,7 +2383,7 @@
       <c r="D79" s="8"/>
       <c r="E79" s="9"/>
     </row>
-    <row r="80" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>45735.722696759258</v>
       </c>
@@ -2378,7 +2396,7 @@
       <c r="D80" s="5"/>
       <c r="E80" s="6"/>
     </row>
-    <row r="81" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="7">
         <v>45735.73709490741</v>
       </c>
@@ -2391,7 +2409,7 @@
       <c r="D81" s="8"/>
       <c r="E81" s="9"/>
     </row>
-    <row r="82" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>45735.791226851848</v>
       </c>
@@ -2404,7 +2422,7 @@
       <c r="D82" s="5"/>
       <c r="E82" s="6"/>
     </row>
-    <row r="83" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A83" s="7">
         <v>45735.815532407411</v>
       </c>
@@ -2417,7 +2435,7 @@
       <c r="D83" s="8"/>
       <c r="E83" s="9"/>
     </row>
-    <row r="84" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>45735.83017361111</v>
       </c>
@@ -2430,7 +2448,7 @@
       <c r="D84" s="5"/>
       <c r="E84" s="6"/>
     </row>
-    <row r="85" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A85" s="7">
         <v>45735.904293981483</v>
       </c>
@@ -2443,7 +2461,7 @@
       <c r="D85" s="8"/>
       <c r="E85" s="9"/>
     </row>
-    <row r="86" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>45735.916076388887</v>
       </c>
@@ -2456,7 +2474,7 @@
       <c r="D86" s="5"/>
       <c r="E86" s="6"/>
     </row>
-    <row r="87" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A87" s="7">
         <v>45735.931064814817</v>
       </c>
@@ -2469,7 +2487,7 @@
       <c r="D87" s="8"/>
       <c r="E87" s="9"/>
     </row>
-    <row r="88" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
         <v>45735.954722222225</v>
       </c>
@@ -2482,7 +2500,7 @@
       <c r="D88" s="5"/>
       <c r="E88" s="6"/>
     </row>
-    <row r="89" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A89" s="7">
         <v>45736.216805555552</v>
       </c>
@@ -2495,7 +2513,7 @@
       <c r="D89" s="8"/>
       <c r="E89" s="9"/>
     </row>
-    <row r="90" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <v>45736.221365740741</v>
       </c>
@@ -2508,7 +2526,7 @@
       <c r="D90" s="5"/>
       <c r="E90" s="6"/>
     </row>
-    <row r="91" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A91" s="7">
         <v>45736.383368055554</v>
       </c>
@@ -2521,7 +2539,7 @@
       <c r="D91" s="8"/>
       <c r="E91" s="9"/>
     </row>
-    <row r="92" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <v>45736.435949074075</v>
       </c>
@@ -2534,7 +2552,7 @@
       <c r="D92" s="5"/>
       <c r="E92" s="6"/>
     </row>
-    <row r="93" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A93" s="7">
         <v>45736.531006944446</v>
       </c>
@@ -2547,7 +2565,7 @@
       <c r="D93" s="8"/>
       <c r="E93" s="9"/>
     </row>
-    <row r="94" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <v>45736.532453703701</v>
       </c>
@@ -2560,7 +2578,7 @@
       <c r="D94" s="5"/>
       <c r="E94" s="6"/>
     </row>
-    <row r="95" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A95" s="7">
         <v>45736.622372685182</v>
       </c>
@@ -2573,7 +2591,7 @@
       <c r="D95" s="8"/>
       <c r="E95" s="9"/>
     </row>
-    <row r="96" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <v>45736.630844907406</v>
       </c>
@@ -2586,7 +2604,7 @@
       <c r="D96" s="5"/>
       <c r="E96" s="6"/>
     </row>
-    <row r="97" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A97" s="7">
         <v>45736.789652777778</v>
       </c>
@@ -2599,7 +2617,7 @@
       <c r="D97" s="8"/>
       <c r="E97" s="9"/>
     </row>
-    <row r="98" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <v>45736.954583333332</v>
       </c>
@@ -2612,7 +2630,7 @@
       <c r="D98" s="5"/>
       <c r="E98" s="6"/>
     </row>
-    <row r="99" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A99" s="7">
         <v>45736.958553240744</v>
       </c>
@@ -2625,7 +2643,7 @@
       <c r="D99" s="8"/>
       <c r="E99" s="9"/>
     </row>
-    <row r="100" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <v>45736.958796296298</v>
       </c>
@@ -2638,7 +2656,7 @@
       <c r="D100" s="5"/>
       <c r="E100" s="6"/>
     </row>
-    <row r="101" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="7">
         <v>45737.594444444447</v>
       </c>
@@ -2651,7 +2669,7 @@
       <c r="D101" s="8"/>
       <c r="E101" s="9"/>
     </row>
-    <row r="102" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <v>45737.594560185185</v>
       </c>
@@ -2664,7 +2682,7 @@
       <c r="D102" s="5"/>
       <c r="E102" s="6"/>
     </row>
-    <row r="103" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="7">
         <v>45737.594675925924</v>
       </c>
@@ -2677,7 +2695,7 @@
       <c r="D103" s="8"/>
       <c r="E103" s="9"/>
     </row>
-    <row r="104" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
         <v>45737.625115740739</v>
       </c>
@@ -2690,7 +2708,7 @@
       <c r="D104" s="5"/>
       <c r="E104" s="6"/>
     </row>
-    <row r="105" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A105" s="7">
         <v>45737.638344907406</v>
       </c>
@@ -2703,7 +2721,7 @@
       <c r="D105" s="8"/>
       <c r="E105" s="9"/>
     </row>
-    <row r="106" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A106" s="4">
         <v>45737.638645833336</v>
       </c>
@@ -2716,7 +2734,7 @@
       <c r="D106" s="5"/>
       <c r="E106" s="6"/>
     </row>
-    <row r="107" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A107" s="7">
         <v>45737.662002314813</v>
       </c>
@@ -2729,7 +2747,7 @@
       <c r="D107" s="8"/>
       <c r="E107" s="9"/>
     </row>
-    <row r="108" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A108" s="4">
         <v>45737.693680555552</v>
       </c>
@@ -2742,7 +2760,7 @@
       <c r="D108" s="5"/>
       <c r="E108" s="6"/>
     </row>
-    <row r="109" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A109" s="7">
         <v>45737.693831018521</v>
       </c>
@@ -2755,7 +2773,7 @@
       <c r="D109" s="8"/>
       <c r="E109" s="9"/>
     </row>
-    <row r="110" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A110" s="4">
         <v>45737.7031712963</v>
       </c>
@@ -2768,7 +2786,7 @@
       <c r="D110" s="5"/>
       <c r="E110" s="6"/>
     </row>
-    <row r="111" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A111" s="7">
         <v>45737.703530092593</v>
       </c>
@@ -2781,7 +2799,7 @@
       <c r="D111" s="8"/>
       <c r="E111" s="9"/>
     </row>
-    <row r="112" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A112" s="4">
         <v>45737.87636574074</v>
       </c>
@@ -2794,7 +2812,7 @@
       <c r="D112" s="5"/>
       <c r="E112" s="6"/>
     </row>
-    <row r="113" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A113" s="7">
         <v>45737.876574074071</v>
       </c>
@@ -2807,7 +2825,7 @@
       <c r="D113" s="8"/>
       <c r="E113" s="9"/>
     </row>
-    <row r="114" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A114" s="4">
         <v>45737.987118055556</v>
       </c>
@@ -2820,7 +2838,7 @@
       <c r="D114" s="5"/>
       <c r="E114" s="6"/>
     </row>
-    <row r="115" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A115" s="7">
         <v>45738.049212962964</v>
       </c>
@@ -2833,7 +2851,7 @@
       <c r="D115" s="8"/>
       <c r="E115" s="9"/>
     </row>
-    <row r="116" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A116" s="4">
         <v>45738.637048611112</v>
       </c>
@@ -2846,7 +2864,7 @@
       <c r="D116" s="5"/>
       <c r="E116" s="6"/>
     </row>
-    <row r="117" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A117" s="7">
         <v>45738.637326388889</v>
       </c>
@@ -2859,7 +2877,7 @@
       <c r="D117" s="8"/>
       <c r="E117" s="9"/>
     </row>
-    <row r="118" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A118" s="4">
         <v>45738.740254629629</v>
       </c>
@@ -2872,7 +2890,7 @@
       <c r="D118" s="5"/>
       <c r="E118" s="6"/>
     </row>
-    <row r="119" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A119" s="7">
         <v>45738.740439814814</v>
       </c>
@@ -2885,7 +2903,7 @@
       <c r="D119" s="8"/>
       <c r="E119" s="9"/>
     </row>
-    <row r="120" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A120" s="4">
         <v>45738.741099537037</v>
       </c>
@@ -2898,7 +2916,7 @@
       <c r="D120" s="5"/>
       <c r="E120" s="6"/>
     </row>
-    <row r="121" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A121" s="7">
         <v>45739.096574074072</v>
       </c>
@@ -2911,7 +2929,7 @@
       <c r="D121" s="8"/>
       <c r="E121" s="9"/>
     </row>
-    <row r="122" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A122" s="4">
         <v>45739.616539351853</v>
       </c>
@@ -2924,7 +2942,7 @@
       <c r="D122" s="5"/>
       <c r="E122" s="6"/>
     </row>
-    <row r="123" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A123" s="10">
         <v>45740.519872685189</v>
       </c>
@@ -2937,7 +2955,7 @@
       <c r="D123" s="11"/>
       <c r="E123" s="12"/>
     </row>
-    <row r="124" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B124" s="17" t="s">
         <v>161</v>
       </c>
@@ -2945,7 +2963,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B125" s="15" t="s">
         <v>163</v>
       </c>
@@ -2953,7 +2971,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="126" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B126" s="17" t="s">
         <v>165</v>
       </c>
@@ -2961,7 +2979,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="127" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B127" s="24" t="s">
         <v>77</v>
       </c>
@@ -2969,7 +2987,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B128" s="24" t="s">
         <v>168</v>
       </c>
@@ -2977,7 +2995,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
         <v>170</v>
       </c>
@@ -2985,7 +3003,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="130" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>171</v>
       </c>
@@ -2993,7 +3011,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="131" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B131" s="27" t="s">
         <v>5</v>
       </c>
@@ -3001,7 +3019,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="132" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B132" s="29" t="s">
         <v>7</v>
       </c>
@@ -3009,7 +3027,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="133" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B133" s="27" t="s">
         <v>9</v>
       </c>
@@ -3017,7 +3035,7 @@
         <v>30509051400865</v>
       </c>
     </row>
-    <row r="134" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B134" s="29" t="s">
         <v>10</v>
       </c>
@@ -3025,7 +3043,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="135" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B135" s="27" t="s">
         <v>12</v>
       </c>
@@ -3033,7 +3051,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="136" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B136" s="29" t="s">
         <v>13</v>
       </c>
@@ -3041,7 +3059,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="137" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B137" s="27" t="s">
         <v>15</v>
       </c>
@@ -3049,7 +3067,7 @@
         <v>20233360</v>
       </c>
     </row>
-    <row r="138" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B138" s="29" t="s">
         <v>16</v>
       </c>
@@ -3057,7 +3075,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="139" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B139" s="27" t="s">
         <v>13</v>
       </c>
@@ -3065,7 +3083,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="140" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B140" s="29" t="s">
         <v>18</v>
       </c>
@@ -3073,7 +3091,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="141" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B141" s="27" t="s">
         <v>18</v>
       </c>
@@ -3081,7 +3099,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="142" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B142" s="29" t="s">
         <v>13</v>
       </c>
@@ -3089,7 +3107,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="143" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B143" s="27" t="s">
         <v>13</v>
       </c>
@@ -3097,7 +3115,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="144" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B144" s="29" t="s">
         <v>13</v>
       </c>
@@ -3105,7 +3123,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="145" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B145" s="27" t="s">
         <v>13</v>
       </c>
@@ -3113,7 +3131,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="146" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B146" s="29" t="s">
         <v>13</v>
       </c>
@@ -3121,7 +3139,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="147" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B147" s="27" t="s">
         <v>20</v>
       </c>
@@ -3129,13 +3147,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="148" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B148" s="29" t="s">
         <v>22</v>
       </c>
       <c r="C148" s="8"/>
     </row>
-    <row r="149" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B149" s="27" t="s">
         <v>23</v>
       </c>
@@ -3143,7 +3161,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="150" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B150" s="29" t="s">
         <v>15</v>
       </c>
@@ -3151,7 +3169,7 @@
         <v>20233360</v>
       </c>
     </row>
-    <row r="151" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B151" s="27" t="s">
         <v>15</v>
       </c>
@@ -3159,7 +3177,7 @@
         <v>20233360</v>
       </c>
     </row>
-    <row r="152" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B152" s="29" t="s">
         <v>15</v>
       </c>
@@ -3167,7 +3185,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="153" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B153" s="27" t="s">
         <v>26</v>
       </c>
@@ -3175,7 +3193,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="154" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B154" s="29" t="s">
         <v>28</v>
       </c>
@@ -3183,7 +3201,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="155" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B155" s="27" t="s">
         <v>30</v>
       </c>
@@ -3191,7 +3209,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="156" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B156" s="29" t="s">
         <v>30</v>
       </c>
@@ -3199,7 +3217,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="157" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B157" s="27" t="s">
         <v>26</v>
       </c>
@@ -3207,7 +3225,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="158" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B158" s="29" t="s">
         <v>32</v>
       </c>
@@ -3215,7 +3233,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="159" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B159" s="27" t="s">
         <v>34</v>
       </c>
@@ -3223,7 +3241,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="160" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B160" s="29" t="s">
         <v>34</v>
       </c>
@@ -3231,7 +3249,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="161" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B161" s="27" t="s">
         <v>26</v>
       </c>
@@ -3239,7 +3257,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="162" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B162" s="29" t="s">
         <v>36</v>
       </c>
@@ -3247,7 +3265,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="163" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B163" s="27" t="s">
         <v>36</v>
       </c>
@@ -3255,7 +3273,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="164" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B164" s="29" t="s">
         <v>34</v>
       </c>
@@ -3263,7 +3281,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="165" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B165" s="27" t="s">
         <v>39</v>
       </c>
@@ -3271,7 +3289,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="166" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B166" s="29" t="s">
         <v>39</v>
       </c>
@@ -3279,7 +3297,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="167" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B167" s="27" t="s">
         <v>41</v>
       </c>
@@ -3287,7 +3305,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="168" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B168" s="29" t="s">
         <v>41</v>
       </c>
@@ -3295,7 +3313,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="169" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B169" s="27" t="s">
         <v>36</v>
       </c>
@@ -3303,7 +3321,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="170" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B170" s="29" t="s">
         <v>15</v>
       </c>
@@ -3311,7 +3329,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="171" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B171" s="27" t="s">
         <v>28</v>
       </c>
@@ -3319,7 +3337,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="172" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B172" s="29" t="s">
         <v>15</v>
       </c>
@@ -3327,7 +3345,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="173" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B173" s="27" t="s">
         <v>28</v>
       </c>
@@ -3335,7 +3353,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="174" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B174" s="29" t="s">
         <v>43</v>
       </c>
@@ -3343,7 +3361,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="175" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B175" s="27" t="s">
         <v>44</v>
       </c>
@@ -3351,7 +3369,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="176" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B176" s="29" t="s">
         <v>41</v>
       </c>
@@ -3359,7 +3377,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="177" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B177" s="27" t="s">
         <v>15</v>
       </c>
@@ -3367,7 +3385,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="178" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B178" s="29" t="s">
         <v>47</v>
       </c>
@@ -3375,7 +3393,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="179" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B179" s="27" t="s">
         <v>49</v>
       </c>
@@ -3383,7 +3401,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="180" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B180" s="29" t="s">
         <v>51</v>
       </c>
@@ -3391,7 +3409,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="181" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B181" s="27" t="s">
         <v>53</v>
       </c>
@@ -3399,7 +3417,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="182" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B182" s="29" t="s">
         <v>55</v>
       </c>
@@ -3407,7 +3425,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="183" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B183" s="27" t="s">
         <v>57</v>
       </c>
@@ -3415,7 +3433,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="184" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B184" s="29" t="s">
         <v>59</v>
       </c>
@@ -3423,7 +3441,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="185" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B185" s="27" t="s">
         <v>61</v>
       </c>
@@ -3431,7 +3449,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="186" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B186" s="29" t="s">
         <v>63</v>
       </c>
@@ -3439,7 +3457,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="187" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B187" s="27" t="s">
         <v>13</v>
       </c>
@@ -3447,7 +3465,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="188" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B188" s="29" t="s">
         <v>65</v>
       </c>
@@ -3455,7 +3473,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="189" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B189" s="27" t="s">
         <v>67</v>
       </c>
@@ -3463,7 +3481,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="190" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B190" s="29" t="s">
         <v>69</v>
       </c>
@@ -3471,7 +3489,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="191" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B191" s="27" t="s">
         <v>71</v>
       </c>
@@ -3479,7 +3497,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="192" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B192" s="29" t="s">
         <v>73</v>
       </c>
@@ -3487,7 +3505,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="193" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B193" s="27" t="s">
         <v>75</v>
       </c>
@@ -3495,7 +3513,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="194" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B194" s="29" t="s">
         <v>77</v>
       </c>
@@ -3503,7 +3521,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="195" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B195" s="27" t="s">
         <v>79</v>
       </c>
@@ -3511,7 +3529,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="196" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B196" s="29" t="s">
         <v>7</v>
       </c>
@@ -3519,7 +3537,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="197" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B197" s="27" t="s">
         <v>82</v>
       </c>
@@ -3527,7 +3545,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="198" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B198" s="29" t="s">
         <v>84</v>
       </c>
@@ -3535,7 +3553,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="199" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B199" s="27" t="s">
         <v>86</v>
       </c>
@@ -3543,7 +3561,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="200" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B200" s="29" t="s">
         <v>88</v>
       </c>
@@ -3551,7 +3569,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="201" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B201" s="27" t="s">
         <v>90</v>
       </c>
@@ -3559,7 +3577,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="202" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B202" s="29" t="s">
         <v>92</v>
       </c>
@@ -3567,7 +3585,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="203" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B203" s="27" t="s">
         <v>94</v>
       </c>
@@ -3575,7 +3593,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="204" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B204" s="29" t="s">
         <v>96</v>
       </c>
@@ -3583,7 +3601,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="205" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B205" s="27" t="s">
         <v>98</v>
       </c>
@@ -3591,7 +3609,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="206" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B206" s="29" t="s">
         <v>100</v>
       </c>
@@ -3599,7 +3617,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="207" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B207" s="27" t="s">
         <v>102</v>
       </c>
@@ -3607,7 +3625,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="208" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B208" s="29" t="s">
         <v>104</v>
       </c>
@@ -3615,7 +3633,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="209" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B209" s="27" t="s">
         <v>106</v>
       </c>
@@ -3623,7 +3641,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="210" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B210" s="29" t="s">
         <v>108</v>
       </c>
@@ -3631,7 +3649,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="211" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B211" s="27" t="s">
         <v>110</v>
       </c>
@@ -3639,7 +3657,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="212" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B212" s="29" t="s">
         <v>112</v>
       </c>
@@ -3647,7 +3665,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="213" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B213" s="27" t="s">
         <v>114</v>
       </c>
@@ -3655,7 +3673,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="214" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B214" s="29" t="s">
         <v>116</v>
       </c>
@@ -3663,7 +3681,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="215" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B215" s="27" t="s">
         <v>118</v>
       </c>
@@ -3671,7 +3689,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="216" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B216" s="29" t="s">
         <v>120</v>
       </c>
@@ -3679,7 +3697,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="217" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B217" s="27" t="s">
         <v>122</v>
       </c>
@@ -3687,7 +3705,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="218" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B218" s="29" t="s">
         <v>88</v>
       </c>
@@ -3695,7 +3713,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="219" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B219" s="27" t="s">
         <v>124</v>
       </c>
@@ -3703,7 +3721,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="220" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B220" s="29" t="s">
         <v>126</v>
       </c>
@@ -3711,7 +3729,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="221" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B221" s="27" t="s">
         <v>128</v>
       </c>
@@ -3719,7 +3737,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="222" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B222" s="29" t="s">
         <v>104</v>
       </c>
@@ -3727,7 +3745,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="223" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B223" s="27" t="s">
         <v>104</v>
       </c>
@@ -3735,7 +3753,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="224" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B224" s="29" t="s">
         <v>131</v>
       </c>
@@ -3743,7 +3761,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="225" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B225" s="27" t="s">
         <v>133</v>
       </c>
@@ -3751,7 +3769,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="226" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B226" s="29" t="s">
         <v>135</v>
       </c>
@@ -3759,7 +3777,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="227" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B227" s="27" t="s">
         <v>137</v>
       </c>
@@ -3767,7 +3785,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="228" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B228" s="29" t="s">
         <v>137</v>
       </c>
@@ -3775,7 +3793,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="229" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B229" s="27" t="s">
         <v>137</v>
       </c>
@@ -3783,7 +3801,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="230" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B230" s="29" t="s">
         <v>139</v>
       </c>
@@ -3791,7 +3809,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="231" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B231" s="27" t="s">
         <v>139</v>
       </c>
@@ -3799,7 +3817,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="232" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B232" s="29" t="s">
         <v>139</v>
       </c>
@@ -3807,7 +3825,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="233" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B233" s="27" t="s">
         <v>141</v>
       </c>
@@ -3815,7 +3833,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="234" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B234" s="29" t="s">
         <v>133</v>
       </c>
@@ -3823,7 +3841,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="235" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B235" s="27" t="s">
         <v>133</v>
       </c>
@@ -3831,7 +3849,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="236" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B236" s="29" t="s">
         <v>79</v>
       </c>
@@ -3839,7 +3857,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="237" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B237" s="27" t="s">
         <v>143</v>
       </c>
@@ -3847,7 +3865,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="238" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B238" s="29" t="s">
         <v>143</v>
       </c>
@@ -3855,7 +3873,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="239" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B239" s="27" t="s">
         <v>146</v>
       </c>
@@ -3863,7 +3881,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="240" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B240" s="29" t="s">
         <v>146</v>
       </c>
@@ -3871,7 +3889,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="241" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B241" s="27" t="s">
         <v>148</v>
       </c>
@@ -3879,7 +3897,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="242" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B242" s="29" t="s">
         <v>148</v>
       </c>
@@ -3887,7 +3905,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="243" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B243" s="27" t="s">
         <v>150</v>
       </c>
@@ -3895,7 +3913,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="244" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B244" s="29" t="s">
         <v>152</v>
       </c>
@@ -3903,7 +3921,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="245" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B245" s="27" t="s">
         <v>154</v>
       </c>
@@ -3911,7 +3929,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="246" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B246" s="29" t="s">
         <v>154</v>
       </c>
@@ -3919,7 +3937,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="247" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B247" s="27" t="s">
         <v>156</v>
       </c>
@@ -3927,7 +3945,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="248" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B248" s="29" t="s">
         <v>156</v>
       </c>
@@ -3935,7 +3953,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="249" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B249" s="27" t="s">
         <v>156</v>
       </c>
@@ -3943,7 +3961,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="250" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B250" s="29" t="s">
         <v>106</v>
       </c>
@@ -3951,7 +3969,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="251" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B251" s="27" t="s">
         <v>158</v>
       </c>
@@ -3959,7 +3977,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="252" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B252" s="29" t="s">
         <v>159</v>
       </c>
@@ -3967,7 +3985,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="253" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B253" s="27" t="s">
         <v>161</v>
       </c>
@@ -3975,7 +3993,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="254" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B254" s="29" t="s">
         <v>163</v>
       </c>
@@ -3983,7 +4001,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="255" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B255" s="27" t="s">
         <v>165</v>
       </c>
@@ -3991,7 +4009,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="256" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B256" s="29" t="s">
         <v>77</v>
       </c>
@@ -3999,7 +4017,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="257" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B257" s="27" t="s">
         <v>173</v>
       </c>
@@ -4007,7 +4025,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="258" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B258" s="29" t="s">
         <v>170</v>
       </c>
@@ -4015,7 +4033,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="259" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B259" s="27" t="s">
         <v>86</v>
       </c>
@@ -4023,7 +4041,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="260" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B260" s="29" t="s">
         <v>86</v>
       </c>
@@ -4031,7 +4049,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="261" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B261" s="27" t="s">
         <v>88</v>
       </c>
@@ -4039,7 +4057,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="262" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B262" s="33" t="s">
         <v>175</v>
       </c>
@@ -4047,7 +4065,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="263" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="263" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B263" s="35" t="s">
         <v>177</v>
       </c>
@@ -4055,12 +4073,36 @@
         <v>178</v>
       </c>
     </row>
-    <row r="264" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="264" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B264" s="26" t="s">
         <v>180</v>
       </c>
       <c r="C264" s="26" t="s">
         <v>179</v>
+      </c>
+    </row>
+    <row r="265" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B265" t="s">
+        <v>181</v>
+      </c>
+      <c r="C265" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="266" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B266" t="s">
+        <v>184</v>
+      </c>
+      <c r="C266" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="267" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B267" t="s">
+        <v>186</v>
+      </c>
+      <c r="C267" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -4269,17 +4311,17 @@
       <selection activeCell="D3" sqref="D3:E134"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="119.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="119.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
@@ -4296,7 +4338,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C3" s="4">
         <v>45724.771736111114</v>
       </c>
@@ -4309,7 +4351,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="7">
         <v>45724.772939814815</v>
       </c>
@@ -4322,7 +4364,7 @@
       <c r="F4" s="8"/>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C5" s="4">
         <v>45724.777685185189</v>
       </c>
@@ -4335,7 +4377,7 @@
       <c r="F5" s="5"/>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C6" s="7">
         <v>45724.783252314817</v>
       </c>
@@ -4348,7 +4390,7 @@
       <c r="F6" s="8"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C7" s="4">
         <v>45724.800636574073</v>
       </c>
@@ -4361,7 +4403,7 @@
       <c r="F7" s="5"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C8" s="7">
         <v>45724.803206018521</v>
       </c>
@@ -4374,7 +4416,7 @@
       <c r="F8" s="8"/>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C9" s="4">
         <v>45724.805752314816</v>
       </c>
@@ -4387,7 +4429,7 @@
       <c r="F9" s="5"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C10" s="7">
         <v>45724.812673611108</v>
       </c>
@@ -4400,7 +4442,7 @@
       <c r="F10" s="8"/>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C11" s="4">
         <v>45725.53019675926</v>
       </c>
@@ -4413,7 +4455,7 @@
       <c r="F11" s="5"/>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C12" s="7">
         <v>45726.039942129632</v>
       </c>
@@ -4426,7 +4468,7 @@
       <c r="F12" s="8"/>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C13" s="4">
         <v>45726.04005787037</v>
       </c>
@@ -4439,7 +4481,7 @@
       <c r="F13" s="5"/>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C14" s="7">
         <v>45726.356793981482</v>
       </c>
@@ -4452,7 +4494,7 @@
       <c r="F14" s="8"/>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C15" s="4">
         <v>45726.357164351852</v>
       </c>
@@ -4465,7 +4507,7 @@
       <c r="F15" s="5"/>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C16" s="7">
         <v>45726.466319444444</v>
       </c>
@@ -4478,7 +4520,7 @@
       <c r="F16" s="8"/>
       <c r="G16" s="9"/>
     </row>
-    <row r="17" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C17" s="4">
         <v>45726.506782407407</v>
       </c>
@@ -4491,7 +4533,7 @@
       <c r="F17" s="5"/>
       <c r="G17" s="6"/>
     </row>
-    <row r="18" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C18" s="7">
         <v>45726.507210648146</v>
       </c>
@@ -4504,7 +4546,7 @@
       <c r="F18" s="8"/>
       <c r="G18" s="9"/>
     </row>
-    <row r="19" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C19" s="4">
         <v>45727.02065972222</v>
       </c>
@@ -4517,7 +4559,7 @@
       <c r="F19" s="5"/>
       <c r="G19" s="6"/>
     </row>
-    <row r="20" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C20" s="7">
         <v>45727.022858796299</v>
       </c>
@@ -4528,7 +4570,7 @@
       <c r="F20" s="8"/>
       <c r="G20" s="9"/>
     </row>
-    <row r="21" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C21" s="4">
         <v>45727.029664351852</v>
       </c>
@@ -4541,7 +4583,7 @@
       <c r="F21" s="5"/>
       <c r="G21" s="6"/>
     </row>
-    <row r="22" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C22" s="7">
         <v>45727.032870370371</v>
       </c>
@@ -4554,7 +4596,7 @@
       <c r="F22" s="8"/>
       <c r="G22" s="9"/>
     </row>
-    <row r="23" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C23" s="4">
         <v>45727.033043981479</v>
       </c>
@@ -4567,7 +4609,7 @@
       <c r="F23" s="5"/>
       <c r="G23" s="6"/>
     </row>
-    <row r="24" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C24" s="7">
         <v>45727.039386574077</v>
       </c>
@@ -4580,7 +4622,7 @@
       <c r="F24" s="8"/>
       <c r="G24" s="9"/>
     </row>
-    <row r="25" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C25" s="4">
         <v>45727.051342592589</v>
       </c>
@@ -4593,7 +4635,7 @@
       <c r="F25" s="5"/>
       <c r="G25" s="6"/>
     </row>
-    <row r="26" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C26" s="7">
         <v>45727.055520833332</v>
       </c>
@@ -4606,7 +4648,7 @@
       <c r="F26" s="8"/>
       <c r="G26" s="9"/>
     </row>
-    <row r="27" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C27" s="4">
         <v>45727.348298611112</v>
       </c>
@@ -4619,7 +4661,7 @@
       <c r="F27" s="5"/>
       <c r="G27" s="6"/>
     </row>
-    <row r="28" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C28" s="7">
         <v>45727.348761574074</v>
       </c>
@@ -4632,7 +4674,7 @@
       <c r="F28" s="8"/>
       <c r="G28" s="9"/>
     </row>
-    <row r="29" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C29" s="4">
         <v>45727.550428240742</v>
       </c>
@@ -4645,7 +4687,7 @@
       <c r="F29" s="5"/>
       <c r="G29" s="6"/>
     </row>
-    <row r="30" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C30" s="7">
         <v>45730.132939814815</v>
       </c>
@@ -4658,7 +4700,7 @@
       <c r="F30" s="8"/>
       <c r="G30" s="9"/>
     </row>
-    <row r="31" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C31" s="4">
         <v>45730.667627314811</v>
       </c>
@@ -4671,7 +4713,7 @@
       <c r="F31" s="5"/>
       <c r="G31" s="6"/>
     </row>
-    <row r="32" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C32" s="7">
         <v>45730.668043981481</v>
       </c>
@@ -4684,7 +4726,7 @@
       <c r="F32" s="8"/>
       <c r="G32" s="9"/>
     </row>
-    <row r="33" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C33" s="4">
         <v>45730.692094907405</v>
       </c>
@@ -4697,7 +4739,7 @@
       <c r="F33" s="5"/>
       <c r="G33" s="6"/>
     </row>
-    <row r="34" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C34" s="7">
         <v>45731.041458333333</v>
       </c>
@@ -4710,7 +4752,7 @@
       <c r="F34" s="8"/>
       <c r="G34" s="9"/>
     </row>
-    <row r="35" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C35" s="4">
         <v>45731.042604166665</v>
       </c>
@@ -4723,7 +4765,7 @@
       <c r="F35" s="5"/>
       <c r="G35" s="6"/>
     </row>
-    <row r="36" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C36" s="7">
         <v>45731.383217592593</v>
       </c>
@@ -4736,7 +4778,7 @@
       <c r="F36" s="8"/>
       <c r="G36" s="9"/>
     </row>
-    <row r="37" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C37" s="4">
         <v>45731.89230324074</v>
       </c>
@@ -4749,7 +4791,7 @@
       <c r="F37" s="5"/>
       <c r="G37" s="6"/>
     </row>
-    <row r="38" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C38" s="7">
         <v>45731.892442129632</v>
       </c>
@@ -4762,7 +4804,7 @@
       <c r="F38" s="8"/>
       <c r="G38" s="9"/>
     </row>
-    <row r="39" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C39" s="4">
         <v>45731.893680555557</v>
       </c>
@@ -4775,7 +4817,7 @@
       <c r="F39" s="5"/>
       <c r="G39" s="6"/>
     </row>
-    <row r="40" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C40" s="7">
         <v>45731.893842592595</v>
       </c>
@@ -4788,7 +4830,7 @@
       <c r="F40" s="8"/>
       <c r="G40" s="9"/>
     </row>
-    <row r="41" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C41" s="4">
         <v>45731.895567129628</v>
       </c>
@@ -4801,7 +4843,7 @@
       <c r="F41" s="5"/>
       <c r="G41" s="6"/>
     </row>
-    <row r="42" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C42" s="7">
         <v>45733.789525462962</v>
       </c>
@@ -4814,7 +4856,7 @@
       <c r="F42" s="8"/>
       <c r="G42" s="9"/>
     </row>
-    <row r="43" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C43" s="4">
         <v>45733.795115740744</v>
       </c>
@@ -4827,7 +4869,7 @@
       <c r="F43" s="5"/>
       <c r="G43" s="6"/>
     </row>
-    <row r="44" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C44" s="7">
         <v>45733.800370370373</v>
       </c>
@@ -4840,7 +4882,7 @@
       <c r="F44" s="8"/>
       <c r="G44" s="9"/>
     </row>
-    <row r="45" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C45" s="4">
         <v>45733.805578703701</v>
       </c>
@@ -4853,7 +4895,7 @@
       <c r="F45" s="5"/>
       <c r="G45" s="6"/>
     </row>
-    <row r="46" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C46" s="7">
         <v>45733.80641203704</v>
       </c>
@@ -4866,7 +4908,7 @@
       <c r="F46" s="8"/>
       <c r="G46" s="9"/>
     </row>
-    <row r="47" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C47" s="4">
         <v>45733.816261574073</v>
       </c>
@@ -4879,7 +4921,7 @@
       <c r="F47" s="5"/>
       <c r="G47" s="6"/>
     </row>
-    <row r="48" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C48" s="7">
         <v>45735.574652777781</v>
       </c>
@@ -4892,7 +4934,7 @@
       <c r="F48" s="8"/>
       <c r="G48" s="9"/>
     </row>
-    <row r="49" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C49" s="4">
         <v>45733.827337962961</v>
       </c>
@@ -4905,7 +4947,7 @@
       <c r="F49" s="5"/>
       <c r="G49" s="6"/>
     </row>
-    <row r="50" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C50" s="7">
         <v>45733.838587962964</v>
       </c>
@@ -4918,7 +4960,7 @@
       <c r="F50" s="8"/>
       <c r="G50" s="9"/>
     </row>
-    <row r="51" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C51" s="4">
         <v>45733.851712962962</v>
       </c>
@@ -4931,7 +4973,7 @@
       <c r="F51" s="5"/>
       <c r="G51" s="6"/>
     </row>
-    <row r="52" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C52" s="7">
         <v>45733.881053240744</v>
       </c>
@@ -4944,7 +4986,7 @@
       <c r="F52" s="8"/>
       <c r="G52" s="9"/>
     </row>
-    <row r="53" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C53" s="4">
         <v>45735.546041666668</v>
       </c>
@@ -4957,7 +4999,7 @@
       <c r="F53" s="5"/>
       <c r="G53" s="6"/>
     </row>
-    <row r="54" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C54" s="7">
         <v>45733.974374999998</v>
       </c>
@@ -4970,7 +5012,7 @@
       <c r="F54" s="8"/>
       <c r="G54" s="9"/>
     </row>
-    <row r="55" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C55" s="4">
         <v>45733.987372685187</v>
       </c>
@@ -4983,7 +5025,7 @@
       <c r="F55" s="5"/>
       <c r="G55" s="6"/>
     </row>
-    <row r="56" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C56" s="7">
         <v>45733.991678240738</v>
       </c>
@@ -4996,7 +5038,7 @@
       <c r="F56" s="8"/>
       <c r="G56" s="9"/>
     </row>
-    <row r="57" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C57" s="4">
         <v>45734.08734953704</v>
       </c>
@@ -5009,7 +5051,7 @@
       <c r="F57" s="5"/>
       <c r="G57" s="6"/>
     </row>
-    <row r="58" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C58" s="7">
         <v>45734.128171296295</v>
       </c>
@@ -5022,7 +5064,7 @@
       <c r="F58" s="8"/>
       <c r="G58" s="9"/>
     </row>
-    <row r="59" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C59" s="4">
         <v>45734.495439814818</v>
       </c>
@@ -5035,7 +5077,7 @@
       <c r="F59" s="5"/>
       <c r="G59" s="6"/>
     </row>
-    <row r="60" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C60" s="7">
         <v>45734.552002314813</v>
       </c>
@@ -5048,7 +5090,7 @@
       <c r="F60" s="8"/>
       <c r="G60" s="9"/>
     </row>
-    <row r="61" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C61" s="4">
         <v>45734.606840277775</v>
       </c>
@@ -5061,7 +5103,7 @@
       <c r="F61" s="5"/>
       <c r="G61" s="6"/>
     </row>
-    <row r="62" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C62" s="7">
         <v>45734.612662037034</v>
       </c>
@@ -5074,7 +5116,7 @@
       <c r="F62" s="8"/>
       <c r="G62" s="9"/>
     </row>
-    <row r="63" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C63" s="4">
         <v>45734.63653935185</v>
       </c>
@@ -5087,7 +5129,7 @@
       <c r="F63" s="5"/>
       <c r="G63" s="6"/>
     </row>
-    <row r="64" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C64" s="7">
         <v>45734.719652777778</v>
       </c>
@@ -5100,7 +5142,7 @@
       <c r="F64" s="8"/>
       <c r="G64" s="9"/>
     </row>
-    <row r="65" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C65" s="4">
         <v>45734.721446759257</v>
       </c>
@@ -5113,7 +5155,7 @@
       <c r="F65" s="5"/>
       <c r="G65" s="6"/>
     </row>
-    <row r="66" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C66" s="7">
         <v>45734.725555555553</v>
       </c>
@@ -5126,7 +5168,7 @@
       <c r="F66" s="8"/>
       <c r="G66" s="9"/>
     </row>
-    <row r="67" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C67" s="4">
         <v>45734.728935185187</v>
       </c>
@@ -5139,7 +5181,7 @@
       <c r="F67" s="5"/>
       <c r="G67" s="6"/>
     </row>
-    <row r="68" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C68" s="7">
         <v>45734.863935185182</v>
       </c>
@@ -5152,7 +5194,7 @@
       <c r="F68" s="8"/>
       <c r="G68" s="9"/>
     </row>
-    <row r="69" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C69" s="4">
         <v>45735.164502314816</v>
       </c>
@@ -5165,7 +5207,7 @@
       <c r="F69" s="5"/>
       <c r="G69" s="6"/>
     </row>
-    <row r="70" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C70" s="7">
         <v>45735.229097222225</v>
       </c>
@@ -5178,7 +5220,7 @@
       <c r="F70" s="8"/>
       <c r="G70" s="9"/>
     </row>
-    <row r="71" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C71" s="4">
         <v>45735.262106481481</v>
       </c>
@@ -5191,7 +5233,7 @@
       <c r="F71" s="5"/>
       <c r="G71" s="6"/>
     </row>
-    <row r="72" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C72" s="7">
         <v>45735.341168981482</v>
       </c>
@@ -5204,7 +5246,7 @@
       <c r="F72" s="8"/>
       <c r="G72" s="9"/>
     </row>
-    <row r="73" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C73" s="4">
         <v>45735.395312499997</v>
       </c>
@@ -5217,7 +5259,7 @@
       <c r="F73" s="5"/>
       <c r="G73" s="6"/>
     </row>
-    <row r="74" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C74" s="7">
         <v>45735.414930555555</v>
       </c>
@@ -5230,7 +5272,7 @@
       <c r="F74" s="8"/>
       <c r="G74" s="9"/>
     </row>
-    <row r="75" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C75" s="4">
         <v>45735.517326388886</v>
       </c>
@@ -5243,7 +5285,7 @@
       <c r="F75" s="5"/>
       <c r="G75" s="6"/>
     </row>
-    <row r="76" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C76" s="7">
         <v>45735.634039351855</v>
       </c>
@@ -5256,7 +5298,7 @@
       <c r="F76" s="8"/>
       <c r="G76" s="9"/>
     </row>
-    <row r="77" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C77" s="4">
         <v>45735.653171296297</v>
       </c>
@@ -5269,7 +5311,7 @@
       <c r="F77" s="5"/>
       <c r="G77" s="6"/>
     </row>
-    <row r="78" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C78" s="7">
         <v>45735.656875000001</v>
       </c>
@@ -5282,7 +5324,7 @@
       <c r="F78" s="8"/>
       <c r="G78" s="9"/>
     </row>
-    <row r="79" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C79" s="4">
         <v>45735.669131944444</v>
       </c>
@@ -5295,7 +5337,7 @@
       <c r="F79" s="5"/>
       <c r="G79" s="6"/>
     </row>
-    <row r="80" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C80" s="7">
         <v>45735.683749999997</v>
       </c>
@@ -5308,7 +5350,7 @@
       <c r="F80" s="8"/>
       <c r="G80" s="9"/>
     </row>
-    <row r="81" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C81" s="4">
         <v>45735.722696759258</v>
       </c>
@@ -5321,7 +5363,7 @@
       <c r="F81" s="5"/>
       <c r="G81" s="6"/>
     </row>
-    <row r="82" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C82" s="7">
         <v>45735.73709490741</v>
       </c>
@@ -5334,7 +5376,7 @@
       <c r="F82" s="8"/>
       <c r="G82" s="9"/>
     </row>
-    <row r="83" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C83" s="4">
         <v>45735.791226851848</v>
       </c>
@@ -5347,7 +5389,7 @@
       <c r="F83" s="5"/>
       <c r="G83" s="6"/>
     </row>
-    <row r="84" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C84" s="7">
         <v>45735.815532407411</v>
       </c>
@@ -5360,7 +5402,7 @@
       <c r="F84" s="8"/>
       <c r="G84" s="9"/>
     </row>
-    <row r="85" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C85" s="4">
         <v>45735.83017361111</v>
       </c>
@@ -5373,7 +5415,7 @@
       <c r="F85" s="5"/>
       <c r="G85" s="6"/>
     </row>
-    <row r="86" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C86" s="7">
         <v>45735.904293981483</v>
       </c>
@@ -5386,7 +5428,7 @@
       <c r="F86" s="8"/>
       <c r="G86" s="9"/>
     </row>
-    <row r="87" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C87" s="4">
         <v>45735.916076388887</v>
       </c>
@@ -5399,7 +5441,7 @@
       <c r="F87" s="5"/>
       <c r="G87" s="6"/>
     </row>
-    <row r="88" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C88" s="7">
         <v>45735.931064814817</v>
       </c>
@@ -5412,7 +5454,7 @@
       <c r="F88" s="8"/>
       <c r="G88" s="9"/>
     </row>
-    <row r="89" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C89" s="4">
         <v>45735.954722222225</v>
       </c>
@@ -5425,7 +5467,7 @@
       <c r="F89" s="5"/>
       <c r="G89" s="6"/>
     </row>
-    <row r="90" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C90" s="7">
         <v>45736.216805555552</v>
       </c>
@@ -5438,7 +5480,7 @@
       <c r="F90" s="8"/>
       <c r="G90" s="9"/>
     </row>
-    <row r="91" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C91" s="4">
         <v>45736.221365740741</v>
       </c>
@@ -5451,7 +5493,7 @@
       <c r="F91" s="5"/>
       <c r="G91" s="6"/>
     </row>
-    <row r="92" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C92" s="7">
         <v>45736.383368055554</v>
       </c>
@@ -5464,7 +5506,7 @@
       <c r="F92" s="8"/>
       <c r="G92" s="9"/>
     </row>
-    <row r="93" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C93" s="4">
         <v>45736.435949074075</v>
       </c>
@@ -5477,7 +5519,7 @@
       <c r="F93" s="5"/>
       <c r="G93" s="6"/>
     </row>
-    <row r="94" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C94" s="7">
         <v>45736.531006944446</v>
       </c>
@@ -5490,7 +5532,7 @@
       <c r="F94" s="8"/>
       <c r="G94" s="9"/>
     </row>
-    <row r="95" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C95" s="4">
         <v>45736.532453703701</v>
       </c>
@@ -5503,7 +5545,7 @@
       <c r="F95" s="5"/>
       <c r="G95" s="6"/>
     </row>
-    <row r="96" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C96" s="7">
         <v>45736.622372685182</v>
       </c>
@@ -5516,7 +5558,7 @@
       <c r="F96" s="8"/>
       <c r="G96" s="9"/>
     </row>
-    <row r="97" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C97" s="4">
         <v>45736.630844907406</v>
       </c>
@@ -5529,7 +5571,7 @@
       <c r="F97" s="5"/>
       <c r="G97" s="6"/>
     </row>
-    <row r="98" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C98" s="7">
         <v>45736.789652777778</v>
       </c>
@@ -5542,7 +5584,7 @@
       <c r="F98" s="8"/>
       <c r="G98" s="9"/>
     </row>
-    <row r="99" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C99" s="4">
         <v>45736.954583333332</v>
       </c>
@@ -5555,7 +5597,7 @@
       <c r="F99" s="5"/>
       <c r="G99" s="6"/>
     </row>
-    <row r="100" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C100" s="7">
         <v>45736.958553240744</v>
       </c>
@@ -5568,7 +5610,7 @@
       <c r="F100" s="8"/>
       <c r="G100" s="9"/>
     </row>
-    <row r="101" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C101" s="4">
         <v>45736.958796296298</v>
       </c>
@@ -5581,7 +5623,7 @@
       <c r="F101" s="5"/>
       <c r="G101" s="6"/>
     </row>
-    <row r="102" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C102" s="7">
         <v>45737.594444444447</v>
       </c>
@@ -5594,7 +5636,7 @@
       <c r="F102" s="8"/>
       <c r="G102" s="9"/>
     </row>
-    <row r="103" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C103" s="4">
         <v>45737.594560185185</v>
       </c>
@@ -5607,7 +5649,7 @@
       <c r="F103" s="5"/>
       <c r="G103" s="6"/>
     </row>
-    <row r="104" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C104" s="7">
         <v>45737.594675925924</v>
       </c>
@@ -5620,7 +5662,7 @@
       <c r="F104" s="8"/>
       <c r="G104" s="9"/>
     </row>
-    <row r="105" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C105" s="4">
         <v>45737.625115740739</v>
       </c>
@@ -5633,7 +5675,7 @@
       <c r="F105" s="5"/>
       <c r="G105" s="6"/>
     </row>
-    <row r="106" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C106" s="7">
         <v>45737.638344907406</v>
       </c>
@@ -5646,7 +5688,7 @@
       <c r="F106" s="8"/>
       <c r="G106" s="9"/>
     </row>
-    <row r="107" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C107" s="4">
         <v>45737.638645833336</v>
       </c>
@@ -5659,7 +5701,7 @@
       <c r="F107" s="5"/>
       <c r="G107" s="6"/>
     </row>
-    <row r="108" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C108" s="7">
         <v>45737.662002314813</v>
       </c>
@@ -5672,7 +5714,7 @@
       <c r="F108" s="8"/>
       <c r="G108" s="9"/>
     </row>
-    <row r="109" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C109" s="4">
         <v>45737.693680555552</v>
       </c>
@@ -5685,7 +5727,7 @@
       <c r="F109" s="5"/>
       <c r="G109" s="6"/>
     </row>
-    <row r="110" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C110" s="7">
         <v>45737.693831018521</v>
       </c>
@@ -5698,7 +5740,7 @@
       <c r="F110" s="8"/>
       <c r="G110" s="9"/>
     </row>
-    <row r="111" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C111" s="4">
         <v>45737.7031712963</v>
       </c>
@@ -5711,7 +5753,7 @@
       <c r="F111" s="5"/>
       <c r="G111" s="6"/>
     </row>
-    <row r="112" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C112" s="7">
         <v>45737.703530092593</v>
       </c>
@@ -5724,7 +5766,7 @@
       <c r="F112" s="8"/>
       <c r="G112" s="9"/>
     </row>
-    <row r="113" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C113" s="4">
         <v>45737.87636574074</v>
       </c>
@@ -5737,7 +5779,7 @@
       <c r="F113" s="5"/>
       <c r="G113" s="6"/>
     </row>
-    <row r="114" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C114" s="7">
         <v>45737.876574074071</v>
       </c>
@@ -5750,7 +5792,7 @@
       <c r="F114" s="8"/>
       <c r="G114" s="9"/>
     </row>
-    <row r="115" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C115" s="4">
         <v>45737.987118055556</v>
       </c>
@@ -5763,7 +5805,7 @@
       <c r="F115" s="5"/>
       <c r="G115" s="6"/>
     </row>
-    <row r="116" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C116" s="7">
         <v>45738.049212962964</v>
       </c>
@@ -5776,7 +5818,7 @@
       <c r="F116" s="8"/>
       <c r="G116" s="9"/>
     </row>
-    <row r="117" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C117" s="4">
         <v>45738.637048611112</v>
       </c>
@@ -5789,7 +5831,7 @@
       <c r="F117" s="5"/>
       <c r="G117" s="6"/>
     </row>
-    <row r="118" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C118" s="7">
         <v>45738.637326388889</v>
       </c>
@@ -5802,7 +5844,7 @@
       <c r="F118" s="8"/>
       <c r="G118" s="9"/>
     </row>
-    <row r="119" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C119" s="4">
         <v>45738.740254629629</v>
       </c>
@@ -5815,7 +5857,7 @@
       <c r="F119" s="5"/>
       <c r="G119" s="6"/>
     </row>
-    <row r="120" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C120" s="7">
         <v>45738.740439814814</v>
       </c>
@@ -5828,7 +5870,7 @@
       <c r="F120" s="8"/>
       <c r="G120" s="9"/>
     </row>
-    <row r="121" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C121" s="4">
         <v>45738.741099537037</v>
       </c>
@@ -5841,7 +5883,7 @@
       <c r="F121" s="5"/>
       <c r="G121" s="6"/>
     </row>
-    <row r="122" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C122" s="7">
         <v>45739.096574074072</v>
       </c>
@@ -5854,7 +5896,7 @@
       <c r="F122" s="8"/>
       <c r="G122" s="9"/>
     </row>
-    <row r="123" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C123" s="4">
         <v>45739.616539351853</v>
       </c>
@@ -5867,7 +5909,7 @@
       <c r="F123" s="5"/>
       <c r="G123" s="6"/>
     </row>
-    <row r="124" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C124" s="7">
         <v>45740.519872685189</v>
       </c>
@@ -5880,7 +5922,7 @@
       <c r="F124" s="8"/>
       <c r="G124" s="9"/>
     </row>
-    <row r="125" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C125" s="4">
         <v>45742.76363425926</v>
       </c>
@@ -5893,7 +5935,7 @@
       <c r="F125" s="5"/>
       <c r="G125" s="6"/>
     </row>
-    <row r="126" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C126" s="7">
         <v>45743.680300925924</v>
       </c>
@@ -5906,7 +5948,7 @@
       <c r="F126" s="8"/>
       <c r="G126" s="9"/>
     </row>
-    <row r="127" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C127" s="4">
         <v>45746.572465277779</v>
       </c>
@@ -5919,7 +5961,7 @@
       <c r="F127" s="5"/>
       <c r="G127" s="6"/>
     </row>
-    <row r="128" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C128" s="7">
         <v>45754.547407407408</v>
       </c>
@@ -5932,7 +5974,7 @@
       <c r="F128" s="8"/>
       <c r="G128" s="9"/>
     </row>
-    <row r="129" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C129" s="4">
         <v>45756.423807870371</v>
       </c>
@@ -5945,7 +5987,7 @@
       <c r="F129" s="5"/>
       <c r="G129" s="6"/>
     </row>
-    <row r="130" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C130" s="7">
         <v>45756.662766203706</v>
       </c>
@@ -5958,7 +6000,7 @@
       <c r="F130" s="8"/>
       <c r="G130" s="9"/>
     </row>
-    <row r="131" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C131" s="4">
         <v>45756.682824074072</v>
       </c>
@@ -5971,7 +6013,7 @@
       <c r="F131" s="5"/>
       <c r="G131" s="6"/>
     </row>
-    <row r="132" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C132" s="7">
         <v>45756.682974537034</v>
       </c>
@@ -5984,7 +6026,7 @@
       <c r="F132" s="8"/>
       <c r="G132" s="9"/>
     </row>
-    <row r="133" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C133" s="4">
         <v>45757.531770833331</v>
       </c>
@@ -5997,7 +6039,7 @@
       <c r="F133" s="5"/>
       <c r="G133" s="6"/>
     </row>
-    <row r="134" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="3:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C134" s="10">
         <v>45759.652187500003</v>
       </c>

</xml_diff>

<commit_message>
Update Record 14-04-2025 07:32
</commit_message>
<xml_diff>
--- a/Records.xlsx
+++ b/Records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zicooo82/Desktop/معهد الوادي/MyWeRepo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3330D30-A684-5742-9CE6-0ECC146A452F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295AFA78-F6D2-C24A-A040-063AB632F6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3460" yWindow="3460" windowWidth="18000" windowHeight="9360" xr2:uid="{AE619845-176D-4C93-91F5-F1442B84480E}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="189">
   <si>
     <t>Timestamp</t>
   </si>
@@ -590,6 +590,12 @@
   </si>
   <si>
     <t>ea20230350@sva.edu.eg</t>
+  </si>
+  <si>
+    <t>https://hagersalim.github.io/myfirstweb/</t>
+  </si>
+  <si>
+    <t>hm20230396@sva.edu.eg</t>
   </si>
 </sst>
 </file>
@@ -1339,10 +1345,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97601210-06D1-436F-9FFC-E5C230996E4C}">
-  <dimension ref="A1:E267"/>
+  <dimension ref="A1:E268"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B261" workbookViewId="0">
-      <selection activeCell="B267" sqref="B267"/>
+      <selection activeCell="B268" sqref="B268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4103,6 +4109,14 @@
       </c>
       <c r="C267" t="s">
         <v>185</v>
+      </c>
+    </row>
+    <row r="268" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B268" t="s">
+        <v>188</v>
+      </c>
+      <c r="C268" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>